<commit_message>
update BLT and MORTRATE
</commit_message>
<xml_diff>
--- a/data/raw/others/BLT.xlsx
+++ b/data/raw/others/BLT.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dev\Documents\GitHub\MMB_forecast_application\data\raw\others\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KaiLong\Documents\GitHub\MMB_forecast_application\data\raw\others\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{806A251C-6135-4BF2-A1D6-60EC2FD7AD3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89447B55-52FD-4921-B8AF-E490CB879525}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataframe" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="354">
   <si>
     <t>BLT_US</t>
   </si>
@@ -1084,9 +1084,6 @@
     <t>1/1/2020</t>
   </si>
   <si>
-    <t>4/1/2020</t>
-  </si>
-  <si>
     <t>BLT_20150223</t>
   </si>
   <si>
@@ -1094,6 +1091,12 @@
   </si>
   <si>
     <t>BLT_20200803</t>
+  </si>
+  <si>
+    <t>2020Q4</t>
+  </si>
+  <si>
+    <t>BLT_20201109</t>
   </si>
 </sst>
 </file>
@@ -1103,7 +1106,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1155,6 +1158,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1191,7 +1202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -1221,6 +1232,7 @@
     <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1603,15 +1615,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E83A3D7-B6BD-4C15-B11E-1920BCD560E3}">
-  <dimension ref="A1:CR108"/>
+  <dimension ref="A1:CS109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="A109" sqref="A109"/>
+    <sheetView tabSelected="1" topLeftCell="BV74" workbookViewId="0">
+      <selection activeCell="CS109" sqref="CS109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="9.140625" style="20"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:97" x14ac:dyDescent="0.25">
       <c r="B1" s="18" t="s">
         <v>150</v>
       </c>
@@ -1895,11 +1911,14 @@
         <v>243</v>
       </c>
       <c r="CR1" s="18" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="2" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+        <v>351</v>
+      </c>
+      <c r="CS1" s="18" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="2" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
         <v>244</v>
       </c>
       <c r="B2">
@@ -2187,9 +2206,12 @@
       <c r="CR2">
         <v>-8.8699999999999992</v>
       </c>
-    </row>
-    <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="CS2">
+        <v>-8.8699999999999992</v>
+      </c>
+    </row>
+    <row r="3" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
         <v>245</v>
       </c>
       <c r="B3">
@@ -2477,9 +2499,12 @@
       <c r="CR3">
         <v>-8.8324999999999996</v>
       </c>
-    </row>
-    <row r="4" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="CS3">
+        <v>-8.8324999999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
         <v>246</v>
       </c>
       <c r="B4">
@@ -2767,9 +2792,12 @@
       <c r="CR4">
         <v>-5.6375000000000002</v>
       </c>
-    </row>
-    <row r="5" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+      <c r="CS4">
+        <v>-5.6375000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
         <v>247</v>
       </c>
       <c r="B5">
@@ -3057,9 +3085,12 @@
       <c r="CR5">
         <v>-10.862500000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+      <c r="CS5">
+        <v>-10.862500000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
         <v>248</v>
       </c>
       <c r="B6">
@@ -3347,9 +3378,12 @@
       <c r="CR6">
         <v>-3.375</v>
       </c>
-    </row>
-    <row r="7" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
+      <c r="CS6">
+        <v>-3.375</v>
+      </c>
+    </row>
+    <row r="7" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
         <v>249</v>
       </c>
       <c r="B7">
@@ -3637,9 +3671,12 @@
       <c r="CR7">
         <v>-4.6825000000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
+      <c r="CS7">
+        <v>-4.6825000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
         <v>250</v>
       </c>
       <c r="B8">
@@ -3927,9 +3964,12 @@
       <c r="CR8">
         <v>-1.2175</v>
       </c>
-    </row>
-    <row r="9" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
+      <c r="CS8">
+        <v>-1.2175</v>
+      </c>
+    </row>
+    <row r="9" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
         <v>251</v>
       </c>
       <c r="B9">
@@ -4217,9 +4257,12 @@
       <c r="CR9">
         <v>1.1325000000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
+      <c r="CS9">
+        <v>1.1325000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
         <v>252</v>
       </c>
       <c r="B10">
@@ -4507,9 +4550,12 @@
       <c r="CR10">
         <v>5.9450000000000003</v>
       </c>
-    </row>
-    <row r="11" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
+      <c r="CS10">
+        <v>5.9450000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A11" s="19" t="s">
         <v>253</v>
       </c>
       <c r="B11">
@@ -4797,9 +4843,12 @@
       <c r="CR11">
         <v>2.4500000000000002</v>
       </c>
-    </row>
-    <row r="12" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
+      <c r="CS11">
+        <v>2.4500000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A12" s="19" t="s">
         <v>254</v>
       </c>
       <c r="B12">
@@ -5087,9 +5136,12 @@
       <c r="CR12">
         <v>1.0249999999999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
+      <c r="CS12">
+        <v>1.0249999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A13" s="19" t="s">
         <v>255</v>
       </c>
       <c r="B13">
@@ -5377,9 +5429,12 @@
       <c r="CR13">
         <v>-4.45</v>
       </c>
-    </row>
-    <row r="14" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
+      <c r="CS13">
+        <v>-4.45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A14" s="19" t="s">
         <v>256</v>
       </c>
       <c r="B14">
@@ -5667,9 +5722,12 @@
       <c r="CR14">
         <v>-2.1875</v>
       </c>
-    </row>
-    <row r="15" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
+      <c r="CS14">
+        <v>-2.1875</v>
+      </c>
+    </row>
+    <row r="15" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A15" s="19" t="s">
         <v>257</v>
       </c>
       <c r="C15">
@@ -5954,9 +6012,12 @@
       <c r="CR15">
         <v>-4.3624999999999998</v>
       </c>
-    </row>
-    <row r="16" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
+      <c r="CS15">
+        <v>-4.3624999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A16" s="19" t="s">
         <v>258</v>
       </c>
       <c r="D16">
@@ -6238,9 +6299,12 @@
       <c r="CR16">
         <v>-5.25</v>
       </c>
-    </row>
-    <row r="17" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A17" s="18" t="s">
+      <c r="CS16">
+        <v>-5.25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A17" s="19" t="s">
         <v>259</v>
       </c>
       <c r="E17">
@@ -6519,9 +6583,12 @@
       <c r="CR17">
         <v>-4.3499999999999996</v>
       </c>
-    </row>
-    <row r="18" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A18" s="18" t="s">
+      <c r="CS17">
+        <v>-4.3499999999999996</v>
+      </c>
+    </row>
+    <row r="18" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A18" s="19" t="s">
         <v>260</v>
       </c>
       <c r="F18">
@@ -6797,9 +6864,12 @@
       <c r="CR18">
         <v>-0.875</v>
       </c>
-    </row>
-    <row r="19" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A19" s="18" t="s">
+      <c r="CS18">
+        <v>-0.875</v>
+      </c>
+    </row>
+    <row r="19" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A19" s="19" t="s">
         <v>261</v>
       </c>
       <c r="G19">
@@ -7072,9 +7142,12 @@
       <c r="CR19">
         <v>-5.4749999999999996</v>
       </c>
-    </row>
-    <row r="20" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A20" s="18" t="s">
+      <c r="CS19">
+        <v>-5.4749999999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A20" s="19" t="s">
         <v>262</v>
       </c>
       <c r="H20">
@@ -7344,9 +7417,12 @@
       <c r="CR20">
         <v>-1.3</v>
       </c>
-    </row>
-    <row r="21" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A21" s="18" t="s">
+      <c r="CS20">
+        <v>-1.3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A21" s="19" t="s">
         <v>263</v>
       </c>
       <c r="I21">
@@ -7613,9 +7689,12 @@
       <c r="CR21">
         <v>23.925000000000001</v>
       </c>
-    </row>
-    <row r="22" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A22" s="18" t="s">
+      <c r="CS21">
+        <v>23.925000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A22" s="19" t="s">
         <v>264</v>
       </c>
       <c r="J22">
@@ -7879,9 +7958,12 @@
       <c r="CR22">
         <v>6.9749999999999996</v>
       </c>
-    </row>
-    <row r="23" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A23" s="18" t="s">
+      <c r="CS22">
+        <v>6.9749999999999996</v>
+      </c>
+    </row>
+    <row r="23" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A23" s="19" t="s">
         <v>265</v>
       </c>
       <c r="K23">
@@ -8142,9 +8224,12 @@
       <c r="CR23">
         <v>5.85</v>
       </c>
-    </row>
-    <row r="24" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A24" s="18" t="s">
+      <c r="CS23">
+        <v>5.85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A24" s="19" t="s">
         <v>266</v>
       </c>
       <c r="L24">
@@ -8402,9 +8487,12 @@
       <c r="CR24">
         <v>3.5750000000000002</v>
       </c>
-    </row>
-    <row r="25" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A25" s="18" t="s">
+      <c r="CS24">
+        <v>3.5750000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A25" s="19" t="s">
         <v>267</v>
       </c>
       <c r="M25">
@@ -8659,9 +8747,12 @@
       <c r="CR25">
         <v>4.5250000000000004</v>
       </c>
-    </row>
-    <row r="26" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A26" s="18" t="s">
+      <c r="CS25">
+        <v>4.5250000000000004</v>
+      </c>
+    </row>
+    <row r="26" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A26" s="19" t="s">
         <v>268</v>
       </c>
       <c r="N26">
@@ -8913,9 +9004,12 @@
       <c r="CR26">
         <v>7.3250000000000002</v>
       </c>
-    </row>
-    <row r="27" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A27" s="18" t="s">
+      <c r="CS26">
+        <v>7.3250000000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A27" s="19" t="s">
         <v>269</v>
       </c>
       <c r="O27">
@@ -9164,9 +9258,12 @@
       <c r="CR27">
         <v>15.45</v>
       </c>
-    </row>
-    <row r="28" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A28" s="18" t="s">
+      <c r="CS27">
+        <v>15.45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A28" s="19" t="s">
         <v>270</v>
       </c>
       <c r="P28">
@@ -9412,9 +9509,12 @@
       <c r="CR28">
         <v>22.4</v>
       </c>
-    </row>
-    <row r="29" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A29" s="18" t="s">
+      <c r="CS28">
+        <v>22.4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A29" s="19" t="s">
         <v>271</v>
       </c>
       <c r="Q29">
@@ -9657,9 +9757,12 @@
       <c r="CR29">
         <v>24.35</v>
       </c>
-    </row>
-    <row r="30" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A30" s="18" t="s">
+      <c r="CS29">
+        <v>24.35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A30" s="19" t="s">
         <v>272</v>
       </c>
       <c r="R30">
@@ -9899,9 +10002,12 @@
       <c r="CR30">
         <v>37.424999999999997</v>
       </c>
-    </row>
-    <row r="31" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A31" s="18" t="s">
+      <c r="CS30">
+        <v>37.424999999999997</v>
+      </c>
+    </row>
+    <row r="31" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A31" s="19" t="s">
         <v>273</v>
       </c>
       <c r="S31">
@@ -10138,9 +10244,12 @@
       <c r="CR31">
         <v>33.225000000000001</v>
       </c>
-    </row>
-    <row r="32" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A32" s="18" t="s">
+      <c r="CS31">
+        <v>33.225000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A32" s="19" t="s">
         <v>274</v>
       </c>
       <c r="T32">
@@ -10374,9 +10483,12 @@
       <c r="CR32">
         <v>29.6</v>
       </c>
-    </row>
-    <row r="33" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A33" s="18" t="s">
+      <c r="CS32">
+        <v>29.6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A33" s="19" t="s">
         <v>275</v>
       </c>
       <c r="U33">
@@ -10607,9 +10719,12 @@
       <c r="CR33">
         <v>34.950000000000003</v>
       </c>
-    </row>
-    <row r="34" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A34" s="18" t="s">
+      <c r="CS33">
+        <v>34.950000000000003</v>
+      </c>
+    </row>
+    <row r="34" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A34" s="19" t="s">
         <v>276</v>
       </c>
       <c r="V34">
@@ -10837,9 +10952,12 @@
       <c r="CR34">
         <v>33.85</v>
       </c>
-    </row>
-    <row r="35" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A35" s="18" t="s">
+      <c r="CS34">
+        <v>33.85</v>
+      </c>
+    </row>
+    <row r="35" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A35" s="19" t="s">
         <v>277</v>
       </c>
       <c r="W35">
@@ -11064,9 +11182,12 @@
       <c r="CR35">
         <v>18.074999999999999</v>
       </c>
-    </row>
-    <row r="36" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A36" s="18" t="s">
+      <c r="CS35">
+        <v>18.074999999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A36" s="19" t="s">
         <v>278</v>
       </c>
       <c r="X36">
@@ -11288,9 +11409,12 @@
       <c r="CR36">
         <v>14.074999999999999</v>
       </c>
-    </row>
-    <row r="37" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A37" s="18" t="s">
+      <c r="CS36">
+        <v>14.074999999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A37" s="19" t="s">
         <v>279</v>
       </c>
       <c r="Y37">
@@ -11509,9 +11633,12 @@
       <c r="CR37">
         <v>17.600000000000001</v>
       </c>
-    </row>
-    <row r="38" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A38" s="18" t="s">
+      <c r="CS37">
+        <v>17.600000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A38" s="19" t="s">
         <v>280</v>
       </c>
       <c r="Z38">
@@ -11727,9 +11854,12 @@
       <c r="CR38">
         <v>15.125</v>
       </c>
-    </row>
-    <row r="39" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A39" s="18" t="s">
+      <c r="CS38">
+        <v>15.125</v>
+      </c>
+    </row>
+    <row r="39" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A39" s="19" t="s">
         <v>281</v>
       </c>
       <c r="AA39">
@@ -11942,9 +12072,12 @@
       <c r="CR39">
         <v>11.275</v>
       </c>
-    </row>
-    <row r="40" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A40" s="18" t="s">
+      <c r="CS39">
+        <v>11.275</v>
+      </c>
+    </row>
+    <row r="40" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A40" s="19" t="s">
         <v>282</v>
       </c>
       <c r="AB40">
@@ -12154,9 +12287,12 @@
       <c r="CR40">
         <v>5.6749999999999998</v>
       </c>
-    </row>
-    <row r="41" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A41" s="18" t="s">
+      <c r="CS40">
+        <v>5.6749999999999998</v>
+      </c>
+    </row>
+    <row r="41" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A41" s="19" t="s">
         <v>283</v>
       </c>
       <c r="AC41">
@@ -12363,9 +12499,12 @@
       <c r="CR41">
         <v>-0.45</v>
       </c>
-    </row>
-    <row r="42" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A42" s="18" t="s">
+      <c r="CS41">
+        <v>-0.45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A42" s="19" t="s">
         <v>284</v>
       </c>
       <c r="AD42">
@@ -12569,9 +12708,12 @@
       <c r="CR42">
         <v>-9.0500000000000007</v>
       </c>
-    </row>
-    <row r="43" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A43" s="18" t="s">
+      <c r="CS42">
+        <v>-9.0500000000000007</v>
+      </c>
+    </row>
+    <row r="43" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A43" s="19" t="s">
         <v>285</v>
       </c>
       <c r="AE43">
@@ -12772,9 +12914,12 @@
       <c r="CR43">
         <v>-15.324999999999999</v>
       </c>
-    </row>
-    <row r="44" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A44" s="18" t="s">
+      <c r="CS43">
+        <v>-15.324999999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A44" s="19" t="s">
         <v>286</v>
       </c>
       <c r="AF44">
@@ -12972,9 +13117,12 @@
       <c r="CR44">
         <v>-9.6</v>
       </c>
-    </row>
-    <row r="45" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A45" s="18" t="s">
+      <c r="CS44">
+        <v>-9.6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A45" s="19" t="s">
         <v>287</v>
       </c>
       <c r="AG45">
@@ -13169,9 +13317,12 @@
       <c r="CR45">
         <v>-13.725</v>
       </c>
-    </row>
-    <row r="46" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A46" s="18" t="s">
+      <c r="CS45">
+        <v>-13.725</v>
+      </c>
+    </row>
+    <row r="46" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A46" s="19" t="s">
         <v>288</v>
       </c>
       <c r="AH46">
@@ -13363,9 +13514,12 @@
       <c r="CR46">
         <v>-17</v>
       </c>
-    </row>
-    <row r="47" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A47" s="18" t="s">
+      <c r="CS46">
+        <v>-17</v>
+      </c>
+    </row>
+    <row r="47" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A47" s="19" t="s">
         <v>289</v>
       </c>
       <c r="AI47">
@@ -13554,9 +13708,12 @@
       <c r="CR47">
         <v>-18.125</v>
       </c>
-    </row>
-    <row r="48" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A48" s="18" t="s">
+      <c r="CS47">
+        <v>-18.125</v>
+      </c>
+    </row>
+    <row r="48" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A48" s="19" t="s">
         <v>290</v>
       </c>
       <c r="AJ48">
@@ -13742,9 +13899,12 @@
       <c r="CR48">
         <v>-10.175000000000001</v>
       </c>
-    </row>
-    <row r="49" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A49" s="18" t="s">
+      <c r="CS48">
+        <v>-10.175000000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A49" s="19" t="s">
         <v>291</v>
       </c>
       <c r="AK49">
@@ -13927,9 +14087,12 @@
       <c r="CR49">
         <v>-5.75</v>
       </c>
-    </row>
-    <row r="50" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A50" s="18" t="s">
+      <c r="CS49">
+        <v>-5.75</v>
+      </c>
+    </row>
+    <row r="50" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A50" s="19" t="s">
         <v>292</v>
       </c>
       <c r="AL50">
@@ -14109,9 +14272,12 @@
       <c r="CR50">
         <v>-4</v>
       </c>
-    </row>
-    <row r="51" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A51" s="18" t="s">
+      <c r="CS50">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A51" s="19" t="s">
         <v>293</v>
       </c>
       <c r="AM51">
@@ -14288,9 +14454,12 @@
       <c r="CR51">
         <v>-6.7249999999999996</v>
       </c>
-    </row>
-    <row r="52" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A52" s="18" t="s">
+      <c r="CS51">
+        <v>-6.7249999999999996</v>
+      </c>
+    </row>
+    <row r="52" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A52" s="19" t="s">
         <v>294</v>
       </c>
       <c r="AN52">
@@ -14464,9 +14633,12 @@
       <c r="CR52">
         <v>-2.3250000000000002</v>
       </c>
-    </row>
-    <row r="53" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A53" s="18" t="s">
+      <c r="CS52">
+        <v>-2.3250000000000002</v>
+      </c>
+    </row>
+    <row r="53" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A53" s="19" t="s">
         <v>295</v>
       </c>
       <c r="AO53">
@@ -14637,9 +14809,12 @@
       <c r="CR53">
         <v>9.1</v>
       </c>
-    </row>
-    <row r="54" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A54" s="18" t="s">
+      <c r="CS53">
+        <v>9.1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A54" s="19" t="s">
         <v>296</v>
       </c>
       <c r="AP54">
@@ -14807,9 +14982,12 @@
       <c r="CR54">
         <v>12</v>
       </c>
-    </row>
-    <row r="55" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A55" s="18" t="s">
+      <c r="CS54">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="55" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A55" s="19" t="s">
         <v>297</v>
       </c>
       <c r="AQ55">
@@ -14974,9 +15152,12 @@
       <c r="CR55">
         <v>16.841666666666669</v>
       </c>
-    </row>
-    <row r="56" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A56" s="18" t="s">
+      <c r="CS55">
+        <v>16.841666666666669</v>
+      </c>
+    </row>
+    <row r="56" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A56" s="19" t="s">
         <v>298</v>
       </c>
       <c r="AR56">
@@ -15138,9 +15319,12 @@
       <c r="CR56">
         <v>19.30833333333333</v>
       </c>
-    </row>
-    <row r="57" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A57" s="18" t="s">
+      <c r="CS56">
+        <v>19.30833333333333</v>
+      </c>
+    </row>
+    <row r="57" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A57" s="19" t="s">
         <v>299</v>
       </c>
       <c r="AS57">
@@ -15299,9 +15483,12 @@
       <c r="CR57">
         <v>32.725000000000001</v>
       </c>
-    </row>
-    <row r="58" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A58" s="18" t="s">
+      <c r="CS57">
+        <v>32.725000000000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A58" s="19" t="s">
         <v>300</v>
       </c>
       <c r="AT58">
@@ -15457,9 +15644,12 @@
       <c r="CR58">
         <v>53.141666666666673</v>
       </c>
-    </row>
-    <row r="59" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A59" s="18" t="s">
+      <c r="CS58">
+        <v>53.141666666666673</v>
+      </c>
+    </row>
+    <row r="59" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A59" s="19" t="s">
         <v>301</v>
       </c>
       <c r="AU59">
@@ -15612,9 +15802,12 @@
       <c r="CR59">
         <v>64.416666666666657</v>
       </c>
-    </row>
-    <row r="60" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A60" s="18" t="s">
+      <c r="CS59">
+        <v>64.416666666666657</v>
+      </c>
+    </row>
+    <row r="60" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A60" s="19" t="s">
         <v>302</v>
       </c>
       <c r="AV60">
@@ -15764,9 +15957,12 @@
       <c r="CR60">
         <v>71.241666666666674</v>
       </c>
-    </row>
-    <row r="61" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A61" s="18" t="s">
+      <c r="CS60">
+        <v>71.241666666666674</v>
+      </c>
+    </row>
+    <row r="61" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A61" s="19" t="s">
         <v>303</v>
       </c>
       <c r="AW61">
@@ -15913,9 +16109,12 @@
       <c r="CR61">
         <v>82.85</v>
       </c>
-    </row>
-    <row r="62" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A62" s="18" t="s">
+      <c r="CS61">
+        <v>82.85</v>
+      </c>
+    </row>
+    <row r="62" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A62" s="19" t="s">
         <v>304</v>
       </c>
       <c r="AX62">
@@ -16059,9 +16258,12 @@
       <c r="CR62">
         <v>65.241666666666674</v>
       </c>
-    </row>
-    <row r="63" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A63" s="18" t="s">
+      <c r="CS62">
+        <v>65.241666666666674</v>
+      </c>
+    </row>
+    <row r="63" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A63" s="19" t="s">
         <v>305</v>
       </c>
       <c r="AY63">
@@ -16202,9 +16404,12 @@
       <c r="CR63">
         <v>46.391666666666673</v>
       </c>
-    </row>
-    <row r="64" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A64" s="18" t="s">
+      <c r="CS63">
+        <v>46.391666666666673</v>
+      </c>
+    </row>
+    <row r="64" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A64" s="19" t="s">
         <v>306</v>
       </c>
       <c r="AZ64">
@@ -16342,9 +16547,12 @@
       <c r="CR64">
         <v>37.733333333333327</v>
       </c>
-    </row>
-    <row r="65" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A65" s="18" t="s">
+      <c r="CS64">
+        <v>37.733333333333327</v>
+      </c>
+    </row>
+    <row r="65" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A65" s="19" t="s">
         <v>307</v>
       </c>
       <c r="BA65">
@@ -16479,9 +16687,12 @@
       <c r="CR65">
         <v>22.8125</v>
       </c>
-    </row>
-    <row r="66" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A66" s="18" t="s">
+      <c r="CS65">
+        <v>22.8125</v>
+      </c>
+    </row>
+    <row r="66" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A66" s="19" t="s">
         <v>308</v>
       </c>
       <c r="BB66">
@@ -16613,9 +16824,12 @@
       <c r="CR66">
         <v>11.7</v>
       </c>
-    </row>
-    <row r="67" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A67" s="18" t="s">
+      <c r="CS66">
+        <v>11.7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A67" s="19" t="s">
         <v>309</v>
       </c>
       <c r="BC67">
@@ -16744,9 +16958,12 @@
       <c r="CR67">
         <v>2.1875</v>
       </c>
-    </row>
-    <row r="68" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A68" s="18" t="s">
+      <c r="CS67">
+        <v>2.1875</v>
+      </c>
+    </row>
+    <row r="68" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A68" s="19" t="s">
         <v>310</v>
       </c>
       <c r="BD68">
@@ -16872,9 +17089,12 @@
       <c r="CR68">
         <v>-3.274999999999999</v>
       </c>
-    </row>
-    <row r="69" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A69" s="18" t="s">
+      <c r="CS68">
+        <v>-3.274999999999999</v>
+      </c>
+    </row>
+    <row r="69" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A69" s="19" t="s">
         <v>311</v>
       </c>
       <c r="BE69">
@@ -16997,9 +17217,12 @@
       <c r="CR69">
         <v>-1.1499999999999999</v>
       </c>
-    </row>
-    <row r="70" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A70" s="18" t="s">
+      <c r="CS69">
+        <v>-1.1499999999999999</v>
+      </c>
+    </row>
+    <row r="70" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A70" s="19" t="s">
         <v>312</v>
       </c>
       <c r="BF70">
@@ -17119,9 +17342,12 @@
       <c r="CR70">
         <v>-1.2749999999999999</v>
       </c>
-    </row>
-    <row r="71" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A71" s="18" t="s">
+      <c r="CS70">
+        <v>-1.2749999999999999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A71" s="19" t="s">
         <v>313</v>
       </c>
       <c r="BG71">
@@ -17238,9 +17464,12 @@
       <c r="CR71">
         <v>-7.6</v>
       </c>
-    </row>
-    <row r="72" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A72" s="18" t="s">
+      <c r="CS71">
+        <v>-7.6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A72" s="19" t="s">
         <v>314</v>
       </c>
       <c r="BH72">
@@ -17354,9 +17583,12 @@
       <c r="CR72">
         <v>-9.3625000000000007</v>
       </c>
-    </row>
-    <row r="73" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A73" s="18" t="s">
+      <c r="CS72">
+        <v>-9.3625000000000007</v>
+      </c>
+    </row>
+    <row r="73" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A73" s="19" t="s">
         <v>315</v>
       </c>
       <c r="BI73">
@@ -17467,9 +17699,12 @@
       <c r="CR73">
         <v>-3.5249999999999999</v>
       </c>
-    </row>
-    <row r="74" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A74" s="18" t="s">
+      <c r="CS73">
+        <v>-3.5249999999999999</v>
+      </c>
+    </row>
+    <row r="74" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A74" s="19" t="s">
         <v>316</v>
       </c>
       <c r="BJ74">
@@ -17577,9 +17812,12 @@
       <c r="CR74">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="75" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A75" s="18" t="s">
+      <c r="CS74">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A75" s="19" t="s">
         <v>317</v>
       </c>
       <c r="BK75">
@@ -17684,9 +17922,12 @@
       <c r="CR75">
         <v>-3.95</v>
       </c>
-    </row>
-    <row r="76" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A76" s="18" t="s">
+      <c r="CS75">
+        <v>-3.95</v>
+      </c>
+    </row>
+    <row r="76" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A76" s="19" t="s">
         <v>318</v>
       </c>
       <c r="BL76">
@@ -17788,9 +18029,12 @@
       <c r="CR76">
         <v>-5.4083333333333332</v>
       </c>
-    </row>
-    <row r="77" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A77" s="18" t="s">
+      <c r="CS76">
+        <v>-5.4083333333333332</v>
+      </c>
+    </row>
+    <row r="77" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A77" s="19" t="s">
         <v>319</v>
       </c>
       <c r="BM77">
@@ -17889,9 +18133,12 @@
       <c r="CR77">
         <v>-4.9333333333333336</v>
       </c>
-    </row>
-    <row r="78" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A78" s="18" t="s">
+      <c r="CS77">
+        <v>-4.9333333333333336</v>
+      </c>
+    </row>
+    <row r="78" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A78" s="19" t="s">
         <v>320</v>
       </c>
       <c r="BN78">
@@ -17987,9 +18234,12 @@
       <c r="CR78">
         <v>-7.1833333333333336</v>
       </c>
-    </row>
-    <row r="79" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A79" s="18" t="s">
+      <c r="CS78">
+        <v>-7.1833333333333336</v>
+      </c>
+    </row>
+    <row r="79" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A79" s="19" t="s">
         <v>321</v>
       </c>
       <c r="BO79">
@@ -18082,9 +18332,12 @@
       <c r="CR79">
         <v>-15.03333333333333</v>
       </c>
-    </row>
-    <row r="80" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A80" s="18" t="s">
+      <c r="CS79">
+        <v>-15.03333333333333</v>
+      </c>
+    </row>
+    <row r="80" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A80" s="19" t="s">
         <v>322</v>
       </c>
       <c r="BP80">
@@ -18174,9 +18427,12 @@
       <c r="CR80">
         <v>-10.883333333333329</v>
       </c>
-    </row>
-    <row r="81" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A81" s="18" t="s">
+      <c r="CS80">
+        <v>-10.883333333333329</v>
+      </c>
+    </row>
+    <row r="81" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A81" s="19" t="s">
         <v>323</v>
       </c>
       <c r="BQ81">
@@ -18263,9 +18519,12 @@
       <c r="CR81">
         <v>-7.395833333333333</v>
       </c>
-    </row>
-    <row r="82" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A82" s="18" t="s">
+      <c r="CS81">
+        <v>-7.395833333333333</v>
+      </c>
+    </row>
+    <row r="82" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A82" s="19" t="s">
         <v>324</v>
       </c>
       <c r="BR82">
@@ -18349,9 +18608,12 @@
       <c r="CR82">
         <v>-3.7666666666666662</v>
       </c>
-    </row>
-    <row r="83" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A83" s="18" t="s">
+      <c r="CS82">
+        <v>-3.7666666666666662</v>
+      </c>
+    </row>
+    <row r="83" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A83" s="19" t="s">
         <v>325</v>
       </c>
       <c r="BS83">
@@ -18432,9 +18694,12 @@
       <c r="CR83">
         <v>-0.33333333333333298</v>
       </c>
-    </row>
-    <row r="84" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A84" s="18" t="s">
+      <c r="CS83">
+        <v>-0.33333333333333298</v>
+      </c>
+    </row>
+    <row r="84" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A84" s="19" t="s">
         <v>326</v>
       </c>
       <c r="BT84">
@@ -18512,9 +18777,12 @@
       <c r="CR84">
         <v>-8.1083333333333343</v>
       </c>
-    </row>
-    <row r="85" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A85" s="18" t="s">
+      <c r="CS84">
+        <v>-8.1083333333333343</v>
+      </c>
+    </row>
+    <row r="85" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A85" s="19" t="s">
         <v>327</v>
       </c>
       <c r="BU85">
@@ -18589,9 +18857,12 @@
       <c r="CR85">
         <v>-7.4166666666666661</v>
       </c>
-    </row>
-    <row r="86" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A86" s="18" t="s">
+      <c r="CS85">
+        <v>-7.4166666666666661</v>
+      </c>
+    </row>
+    <row r="86" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A86" s="19" t="s">
         <v>328</v>
       </c>
       <c r="BV86">
@@ -18663,9 +18934,12 @@
       <c r="CR86">
         <v>-4.2476190476190476</v>
       </c>
-    </row>
-    <row r="87" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A87" s="18" t="s">
+      <c r="CS86">
+        <v>-4.2476190476190476</v>
+      </c>
+    </row>
+    <row r="87" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A87" s="19" t="s">
         <v>329</v>
       </c>
       <c r="BW87">
@@ -18734,9 +19008,12 @@
       <c r="CR87">
         <v>-3.3142857142857149</v>
       </c>
-    </row>
-    <row r="88" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A88" s="18" t="s">
+      <c r="CS87">
+        <v>-3.3142857142857149</v>
+      </c>
+    </row>
+    <row r="88" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A88" s="19" t="s">
         <v>330</v>
       </c>
       <c r="BX88">
@@ -18802,9 +19079,12 @@
       <c r="CR88">
         <v>-6.7</v>
       </c>
-    </row>
-    <row r="89" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A89" s="18" t="s">
+      <c r="CS88">
+        <v>-6.7</v>
+      </c>
+    </row>
+    <row r="89" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A89" s="19" t="s">
         <v>331</v>
       </c>
       <c r="BY89">
@@ -18867,9 +19147,12 @@
       <c r="CR89">
         <v>3.35952380952381</v>
       </c>
-    </row>
-    <row r="90" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A90" s="18" t="s">
+      <c r="CS89">
+        <v>3.35952380952381</v>
+      </c>
+    </row>
+    <row r="90" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A90" s="19" t="s">
         <v>332</v>
       </c>
       <c r="BZ90">
@@ -18929,9 +19212,12 @@
       <c r="CR90">
         <v>5.4297619047619046</v>
       </c>
-    </row>
-    <row r="91" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A91" s="18" t="s">
+      <c r="CS90">
+        <v>5.4297619047619046</v>
+      </c>
+    </row>
+    <row r="91" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A91" s="19" t="s">
         <v>333</v>
       </c>
       <c r="CA91">
@@ -18988,9 +19274,12 @@
       <c r="CR91">
         <v>8.9749999999999996</v>
       </c>
-    </row>
-    <row r="92" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A92" s="18" t="s">
+      <c r="CS91">
+        <v>8.9749999999999996</v>
+      </c>
+    </row>
+    <row r="92" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A92" s="19" t="s">
         <v>334</v>
       </c>
       <c r="CB92">
@@ -19044,9 +19333,12 @@
       <c r="CR92">
         <v>11.483333333333331</v>
       </c>
-    </row>
-    <row r="93" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A93" s="18" t="s">
+      <c r="CS92">
+        <v>11.483333333333331</v>
+      </c>
+    </row>
+    <row r="93" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A93" s="19" t="s">
         <v>335</v>
       </c>
       <c r="CC93">
@@ -19097,9 +19389,12 @@
       <c r="CR93">
         <v>6.4380952380952383</v>
       </c>
-    </row>
-    <row r="94" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A94" s="18" t="s">
+      <c r="CS93">
+        <v>6.4380952380952383</v>
+      </c>
+    </row>
+    <row r="94" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A94" s="19" t="s">
         <v>336</v>
       </c>
       <c r="CD94">
@@ -19147,9 +19442,12 @@
       <c r="CR94">
         <v>5.8666666666666671</v>
       </c>
-    </row>
-    <row r="95" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A95" s="18" t="s">
+      <c r="CS94">
+        <v>5.8666666666666671</v>
+      </c>
+    </row>
+    <row r="95" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A95" s="19" t="s">
         <v>337</v>
       </c>
       <c r="CE95">
@@ -19194,9 +19492,12 @@
       <c r="CR95">
         <v>4.1392857142857142</v>
       </c>
-    </row>
-    <row r="96" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A96" s="18" t="s">
+      <c r="CS95">
+        <v>4.1392857142857142</v>
+      </c>
+    </row>
+    <row r="96" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A96" s="19" t="s">
         <v>338</v>
       </c>
       <c r="CF96">
@@ -19238,9 +19539,12 @@
       <c r="CR96">
         <v>0.20000000000000021</v>
       </c>
-    </row>
-    <row r="97" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A97" s="18" t="s">
+      <c r="CS96">
+        <v>0.20000000000000021</v>
+      </c>
+    </row>
+    <row r="97" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A97" s="19" t="s">
         <v>339</v>
       </c>
       <c r="CG97">
@@ -19279,9 +19583,12 @@
       <c r="CR97">
         <v>-1.980952380952381</v>
       </c>
-    </row>
-    <row r="98" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A98" s="18" t="s">
+      <c r="CS97">
+        <v>-1.980952380952381</v>
+      </c>
+    </row>
+    <row r="98" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A98" s="19" t="s">
         <v>340</v>
       </c>
       <c r="CH98">
@@ -19317,9 +19624,12 @@
       <c r="CR98">
         <v>-0.79166666666666707</v>
       </c>
-    </row>
-    <row r="99" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A99" s="18" t="s">
+      <c r="CS98">
+        <v>-0.79166666666666707</v>
+      </c>
+    </row>
+    <row r="99" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A99" s="19" t="s">
         <v>341</v>
       </c>
       <c r="CI99">
@@ -19352,9 +19662,12 @@
       <c r="CR99">
         <v>-4.0999999999999996</v>
       </c>
-    </row>
-    <row r="100" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A100" s="18" t="s">
+      <c r="CS99">
+        <v>-4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="100" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A100" s="19" t="s">
         <v>342</v>
       </c>
       <c r="CJ100">
@@ -19384,9 +19697,12 @@
       <c r="CR100">
         <v>-6.5583333333333336</v>
       </c>
-    </row>
-    <row r="101" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A101" s="18" t="s">
+      <c r="CS100">
+        <v>-6.5583333333333336</v>
+      </c>
+    </row>
+    <row r="101" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A101" s="19" t="s">
         <v>343</v>
       </c>
       <c r="CK101">
@@ -19413,9 +19729,12 @@
       <c r="CR101">
         <v>-5.8416666666666668</v>
       </c>
-    </row>
-    <row r="102" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A102" s="18" t="s">
+      <c r="CS101">
+        <v>-5.8416666666666668</v>
+      </c>
+    </row>
+    <row r="102" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A102" s="19" t="s">
         <v>344</v>
       </c>
       <c r="CL102">
@@ -19439,9 +19758,12 @@
       <c r="CR102">
         <v>4.7125000000000004</v>
       </c>
-    </row>
-    <row r="103" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A103" s="18" t="s">
+      <c r="CS102">
+        <v>4.7125000000000004</v>
+      </c>
+    </row>
+    <row r="103" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A103" s="19" t="s">
         <v>345</v>
       </c>
       <c r="CM103">
@@ -19462,9 +19784,12 @@
       <c r="CR103">
         <v>0.7488095238095237</v>
       </c>
-    </row>
-    <row r="104" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A104" s="18" t="s">
+      <c r="CS103">
+        <v>0.7488095238095237</v>
+      </c>
+    </row>
+    <row r="104" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A104" s="19" t="s">
         <v>346</v>
       </c>
       <c r="CN104">
@@ -19482,9 +19807,12 @@
       <c r="CR104">
         <v>-1.33095238095238</v>
       </c>
-    </row>
-    <row r="105" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A105" s="18" t="s">
+      <c r="CS104">
+        <v>-1.33095238095238</v>
+      </c>
+    </row>
+    <row r="105" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A105" s="19" t="s">
         <v>347</v>
       </c>
       <c r="CO105">
@@ -19499,9 +19827,12 @@
       <c r="CR105">
         <v>6.7</v>
       </c>
-    </row>
-    <row r="106" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A106" s="18" t="s">
+      <c r="CS105">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="106" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A106" s="19" t="s">
         <v>348</v>
       </c>
       <c r="CP106">
@@ -19513,10 +19844,13 @@
       <c r="CR106">
         <v>-3.095238095238095E-2</v>
       </c>
-    </row>
-    <row r="107" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A107" s="18" t="s">
-        <v>349</v>
+      <c r="CS106">
+        <v>-3.095238095238095E-2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A107" s="19">
+        <v>43834</v>
       </c>
       <c r="CQ107">
         <v>35.61785714285714</v>
@@ -19524,34 +19858,50 @@
       <c r="CR107">
         <v>35.61785714285714</v>
       </c>
-    </row>
-    <row r="108" spans="1:96" x14ac:dyDescent="0.25">
+      <c r="CS107">
+        <v>35.61785714285714</v>
+      </c>
+    </row>
+    <row r="108" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A108" s="19">
-        <v>44013</v>
+        <v>43840</v>
       </c>
       <c r="CR108">
         <v>68.608333333333334</v>
+      </c>
+      <c r="CS108">
+        <v>68.608333333333334</v>
+      </c>
+    </row>
+    <row r="109" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="CS109">
+        <v>34.885714285714286</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B108"/>
+  <dimension ref="A1:B109"/>
   <sheetViews>
     <sheetView topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="K101" sqref="K101"/>
+      <selection activeCell="B109" sqref="B109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -20408,6 +20758,14 @@
       </c>
       <c r="B108">
         <v>68.608333333333334</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="17">
+        <v>44105</v>
+      </c>
+      <c r="B109">
+        <v>34.885714285714286</v>
       </c>
     </row>
   </sheetData>
@@ -20421,10 +20779,10 @@
   <dimension ref="A1:W140"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="I124" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="I115" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K132" sqref="K132"/>
+      <selection pane="bottomRight" activeCell="K133" sqref="K133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23626,7 +23984,7 @@
         <v>93</v>
       </c>
       <c r="K118" s="6">
-        <f t="shared" ref="K118:K132" si="3">AVERAGE(L118:M118,AVERAGE(N118:P118),AVERAGE(Q118:W118))</f>
+        <f t="shared" ref="K118:K133" si="3">AVERAGE(L118:M118,AVERAGE(N118:P118),AVERAGE(Q118:W118))</f>
         <v>5.8666666666666671</v>
       </c>
       <c r="L118" s="4">
@@ -24404,7 +24762,7 @@
     </row>
     <row r="132" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="K132" s="6">
         <f t="shared" si="3"/>
@@ -24460,7 +24818,61 @@
       </c>
     </row>
     <row r="133" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="O133" s="4"/>
+      <c r="A133" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="K133" s="6">
+        <f t="shared" si="3"/>
+        <v>34.885714285714286</v>
+      </c>
+      <c r="L133" s="4">
+        <f>0+40.6-2.9-0</f>
+        <v>37.700000000000003</v>
+      </c>
+      <c r="M133" s="4">
+        <f>0+34.3-3-0</f>
+        <v>31.299999999999997</v>
+      </c>
+      <c r="N133" s="4">
+        <f>9+49.3-1.5-0</f>
+        <v>56.8</v>
+      </c>
+      <c r="O133" s="4">
+        <f>4.3+52.2-1.4-0</f>
+        <v>55.1</v>
+      </c>
+      <c r="P133" s="4">
+        <f>2.9+43.5-1.4-0</f>
+        <v>45</v>
+      </c>
+      <c r="Q133" s="4">
+        <f>0+13.1-1.6-0</f>
+        <v>11.5</v>
+      </c>
+      <c r="R133" s="4">
+        <f>1.8+9.1-1.8-0</f>
+        <v>9.1</v>
+      </c>
+      <c r="S133" s="4">
+        <f>0+16.1-1.8-0</f>
+        <v>14.3</v>
+      </c>
+      <c r="T133" s="4">
+        <f>3.4+20.3-3.4-0</f>
+        <v>20.3</v>
+      </c>
+      <c r="U133" s="4">
+        <f>3.5+17.5-1.8-0</f>
+        <v>19.2</v>
+      </c>
+      <c r="V133" s="4">
+        <f>0+20-0-0</f>
+        <v>20</v>
+      </c>
+      <c r="W133" s="4">
+        <f>33.3+16.7-16.7-0</f>
+        <v>33.299999999999997</v>
+      </c>
     </row>
     <row r="134" spans="1:23" x14ac:dyDescent="0.25">
       <c r="O134" s="4"/>

</xml_diff>

<commit_message>
Data and code updates for 2021Q1
</commit_message>
<xml_diff>
--- a/data/raw/others/BLT.xlsx
+++ b/data/raw/others/BLT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaspe\Documents\GitHub\MMB_forecast_application\data\raw\others\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dev\Documents\GitHub\MMB_forecast_application\data\raw\others\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9902B1F-08BA-441F-9258-13F111A19887}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22FD9B30-C24F-47F0-A76B-4822AAC46756}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="370" yWindow="460" windowWidth="14130" windowHeight="10340" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataframe" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="355">
   <si>
     <t>BLT_US</t>
   </si>
@@ -1094,6 +1094,12 @@
   </si>
   <si>
     <t>BLT_20201109</t>
+  </si>
+  <si>
+    <t>2021Q1</t>
+  </si>
+  <si>
+    <t>BLT_20210201</t>
   </si>
 </sst>
 </file>
@@ -1612,19 +1618,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E83A3D7-B6BD-4C15-B11E-1920BCD560E3}">
-  <dimension ref="A1:CS109"/>
+  <dimension ref="A1:CT110"/>
   <sheetViews>
-    <sheetView topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="A109" sqref="A109"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="CS110" sqref="CS110"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="9.1796875" style="20"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="9.140625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:97" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:98" x14ac:dyDescent="0.25">
       <c r="B1" s="18" t="s">
         <v>150</v>
       </c>
@@ -1913,8 +1919,11 @@
       <c r="CS1" s="18" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="2" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT1" s="18" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="2" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>244</v>
       </c>
@@ -2206,8 +2215,11 @@
       <c r="CS2">
         <v>-8.8699999999999992</v>
       </c>
-    </row>
-    <row r="3" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT2">
+        <v>-8.8699999999999992</v>
+      </c>
+    </row>
+    <row r="3" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>245</v>
       </c>
@@ -2499,8 +2511,11 @@
       <c r="CS3">
         <v>-8.8324999999999996</v>
       </c>
-    </row>
-    <row r="4" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT3">
+        <v>-8.8324999999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>246</v>
       </c>
@@ -2792,8 +2807,11 @@
       <c r="CS4">
         <v>-5.6375000000000002</v>
       </c>
-    </row>
-    <row r="5" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT4">
+        <v>-5.6375000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>247</v>
       </c>
@@ -3085,8 +3103,11 @@
       <c r="CS5">
         <v>-10.862500000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT5">
+        <v>-10.862500000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>248</v>
       </c>
@@ -3378,8 +3399,11 @@
       <c r="CS6">
         <v>-3.375</v>
       </c>
-    </row>
-    <row r="7" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT6">
+        <v>-3.375</v>
+      </c>
+    </row>
+    <row r="7" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>249</v>
       </c>
@@ -3671,8 +3695,11 @@
       <c r="CS7">
         <v>-4.6825000000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT7">
+        <v>-4.6825000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>250</v>
       </c>
@@ -3964,8 +3991,11 @@
       <c r="CS8">
         <v>-1.2175</v>
       </c>
-    </row>
-    <row r="9" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT8">
+        <v>-1.2175</v>
+      </c>
+    </row>
+    <row r="9" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>251</v>
       </c>
@@ -4257,8 +4287,11 @@
       <c r="CS9">
         <v>1.1325000000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT9">
+        <v>1.1325000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>252</v>
       </c>
@@ -4550,8 +4583,11 @@
       <c r="CS10">
         <v>5.9450000000000003</v>
       </c>
-    </row>
-    <row r="11" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT10">
+        <v>5.9450000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>253</v>
       </c>
@@ -4843,8 +4879,11 @@
       <c r="CS11">
         <v>2.4500000000000002</v>
       </c>
-    </row>
-    <row r="12" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT11">
+        <v>2.4500000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>254</v>
       </c>
@@ -5136,8 +5175,11 @@
       <c r="CS12">
         <v>1.0249999999999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT12">
+        <v>1.0249999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>255</v>
       </c>
@@ -5429,8 +5471,11 @@
       <c r="CS13">
         <v>-4.45</v>
       </c>
-    </row>
-    <row r="14" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT13">
+        <v>-4.45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
         <v>256</v>
       </c>
@@ -5722,8 +5767,11 @@
       <c r="CS14">
         <v>-2.1875</v>
       </c>
-    </row>
-    <row r="15" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT14">
+        <v>-2.1875</v>
+      </c>
+    </row>
+    <row r="15" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>257</v>
       </c>
@@ -6012,8 +6060,11 @@
       <c r="CS15">
         <v>-4.3624999999999998</v>
       </c>
-    </row>
-    <row r="16" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT15">
+        <v>-4.3624999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>258</v>
       </c>
@@ -6299,8 +6350,11 @@
       <c r="CS16">
         <v>-5.25</v>
       </c>
-    </row>
-    <row r="17" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT16">
+        <v>-5.25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
         <v>259</v>
       </c>
@@ -6583,8 +6637,11 @@
       <c r="CS17">
         <v>-4.3499999999999996</v>
       </c>
-    </row>
-    <row r="18" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT17">
+        <v>-4.3499999999999996</v>
+      </c>
+    </row>
+    <row r="18" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
         <v>260</v>
       </c>
@@ -6864,8 +6921,11 @@
       <c r="CS18">
         <v>-0.875</v>
       </c>
-    </row>
-    <row r="19" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT18">
+        <v>-0.875</v>
+      </c>
+    </row>
+    <row r="19" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>261</v>
       </c>
@@ -7142,8 +7202,11 @@
       <c r="CS19">
         <v>-5.4749999999999996</v>
       </c>
-    </row>
-    <row r="20" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT19">
+        <v>-5.4749999999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
         <v>262</v>
       </c>
@@ -7417,8 +7480,11 @@
       <c r="CS20">
         <v>-1.3</v>
       </c>
-    </row>
-    <row r="21" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT20">
+        <v>-1.3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
         <v>263</v>
       </c>
@@ -7689,8 +7755,11 @@
       <c r="CS21">
         <v>23.925000000000001</v>
       </c>
-    </row>
-    <row r="22" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT21">
+        <v>23.925000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
         <v>264</v>
       </c>
@@ -7958,8 +8027,11 @@
       <c r="CS22">
         <v>6.9749999999999996</v>
       </c>
-    </row>
-    <row r="23" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT22">
+        <v>6.9749999999999996</v>
+      </c>
+    </row>
+    <row r="23" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>265</v>
       </c>
@@ -8224,8 +8296,11 @@
       <c r="CS23">
         <v>5.85</v>
       </c>
-    </row>
-    <row r="24" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT23">
+        <v>5.85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
         <v>266</v>
       </c>
@@ -8487,8 +8562,11 @@
       <c r="CS24">
         <v>3.5750000000000002</v>
       </c>
-    </row>
-    <row r="25" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT24">
+        <v>3.5750000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
         <v>267</v>
       </c>
@@ -8747,8 +8825,11 @@
       <c r="CS25">
         <v>4.5250000000000004</v>
       </c>
-    </row>
-    <row r="26" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT25">
+        <v>4.5250000000000004</v>
+      </c>
+    </row>
+    <row r="26" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
         <v>268</v>
       </c>
@@ -9004,8 +9085,11 @@
       <c r="CS26">
         <v>7.3250000000000002</v>
       </c>
-    </row>
-    <row r="27" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT26">
+        <v>7.3250000000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A27" s="19" t="s">
         <v>269</v>
       </c>
@@ -9258,8 +9342,11 @@
       <c r="CS27">
         <v>15.45</v>
       </c>
-    </row>
-    <row r="28" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT27">
+        <v>15.45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A28" s="19" t="s">
         <v>270</v>
       </c>
@@ -9509,8 +9596,11 @@
       <c r="CS28">
         <v>22.4</v>
       </c>
-    </row>
-    <row r="29" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT28">
+        <v>22.4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A29" s="19" t="s">
         <v>271</v>
       </c>
@@ -9757,8 +9847,11 @@
       <c r="CS29">
         <v>24.35</v>
       </c>
-    </row>
-    <row r="30" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT29">
+        <v>24.35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
         <v>272</v>
       </c>
@@ -10002,8 +10095,11 @@
       <c r="CS30">
         <v>37.424999999999997</v>
       </c>
-    </row>
-    <row r="31" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT30">
+        <v>37.424999999999997</v>
+      </c>
+    </row>
+    <row r="31" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
         <v>273</v>
       </c>
@@ -10244,8 +10340,11 @@
       <c r="CS31">
         <v>33.225000000000001</v>
       </c>
-    </row>
-    <row r="32" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT31">
+        <v>33.225000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A32" s="19" t="s">
         <v>274</v>
       </c>
@@ -10483,8 +10582,11 @@
       <c r="CS32">
         <v>29.6</v>
       </c>
-    </row>
-    <row r="33" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT32">
+        <v>29.6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
         <v>275</v>
       </c>
@@ -10719,8 +10821,11 @@
       <c r="CS33">
         <v>34.950000000000003</v>
       </c>
-    </row>
-    <row r="34" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT33">
+        <v>34.950000000000003</v>
+      </c>
+    </row>
+    <row r="34" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
         <v>276</v>
       </c>
@@ -10952,8 +11057,11 @@
       <c r="CS34">
         <v>33.85</v>
       </c>
-    </row>
-    <row r="35" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT34">
+        <v>33.85</v>
+      </c>
+    </row>
+    <row r="35" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
         <v>277</v>
       </c>
@@ -11182,8 +11290,11 @@
       <c r="CS35">
         <v>18.074999999999999</v>
       </c>
-    </row>
-    <row r="36" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT35">
+        <v>18.074999999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A36" s="19" t="s">
         <v>278</v>
       </c>
@@ -11409,8 +11520,11 @@
       <c r="CS36">
         <v>14.074999999999999</v>
       </c>
-    </row>
-    <row r="37" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT36">
+        <v>14.074999999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A37" s="19" t="s">
         <v>279</v>
       </c>
@@ -11633,8 +11747,11 @@
       <c r="CS37">
         <v>17.600000000000001</v>
       </c>
-    </row>
-    <row r="38" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT37">
+        <v>17.600000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A38" s="19" t="s">
         <v>280</v>
       </c>
@@ -11854,8 +11971,11 @@
       <c r="CS38">
         <v>15.125</v>
       </c>
-    </row>
-    <row r="39" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT38">
+        <v>15.125</v>
+      </c>
+    </row>
+    <row r="39" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A39" s="19" t="s">
         <v>281</v>
       </c>
@@ -12072,8 +12192,11 @@
       <c r="CS39">
         <v>11.275</v>
       </c>
-    </row>
-    <row r="40" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT39">
+        <v>11.275</v>
+      </c>
+    </row>
+    <row r="40" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A40" s="19" t="s">
         <v>282</v>
       </c>
@@ -12287,8 +12410,11 @@
       <c r="CS40">
         <v>5.6749999999999998</v>
       </c>
-    </row>
-    <row r="41" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT40">
+        <v>5.6749999999999998</v>
+      </c>
+    </row>
+    <row r="41" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A41" s="19" t="s">
         <v>283</v>
       </c>
@@ -12499,8 +12625,11 @@
       <c r="CS41">
         <v>-0.45</v>
       </c>
-    </row>
-    <row r="42" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT41">
+        <v>-0.45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A42" s="19" t="s">
         <v>284</v>
       </c>
@@ -12708,8 +12837,11 @@
       <c r="CS42">
         <v>-9.0500000000000007</v>
       </c>
-    </row>
-    <row r="43" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT42">
+        <v>-9.0500000000000007</v>
+      </c>
+    </row>
+    <row r="43" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A43" s="19" t="s">
         <v>285</v>
       </c>
@@ -12914,8 +13046,11 @@
       <c r="CS43">
         <v>-15.324999999999999</v>
       </c>
-    </row>
-    <row r="44" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT43">
+        <v>-15.324999999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A44" s="19" t="s">
         <v>286</v>
       </c>
@@ -13117,8 +13252,11 @@
       <c r="CS44">
         <v>-9.6</v>
       </c>
-    </row>
-    <row r="45" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT44">
+        <v>-9.6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A45" s="19" t="s">
         <v>287</v>
       </c>
@@ -13317,8 +13455,11 @@
       <c r="CS45">
         <v>-13.725</v>
       </c>
-    </row>
-    <row r="46" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT45">
+        <v>-13.725</v>
+      </c>
+    </row>
+    <row r="46" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A46" s="19" t="s">
         <v>288</v>
       </c>
@@ -13514,8 +13655,11 @@
       <c r="CS46">
         <v>-17</v>
       </c>
-    </row>
-    <row r="47" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT46">
+        <v>-17</v>
+      </c>
+    </row>
+    <row r="47" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A47" s="19" t="s">
         <v>289</v>
       </c>
@@ -13708,8 +13852,11 @@
       <c r="CS47">
         <v>-18.125</v>
       </c>
-    </row>
-    <row r="48" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT47">
+        <v>-18.125</v>
+      </c>
+    </row>
+    <row r="48" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A48" s="19" t="s">
         <v>290</v>
       </c>
@@ -13899,8 +14046,11 @@
       <c r="CS48">
         <v>-10.175000000000001</v>
       </c>
-    </row>
-    <row r="49" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT48">
+        <v>-10.175000000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A49" s="19" t="s">
         <v>291</v>
       </c>
@@ -14087,8 +14237,11 @@
       <c r="CS49">
         <v>-5.75</v>
       </c>
-    </row>
-    <row r="50" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT49">
+        <v>-5.75</v>
+      </c>
+    </row>
+    <row r="50" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A50" s="19" t="s">
         <v>292</v>
       </c>
@@ -14272,8 +14425,11 @@
       <c r="CS50">
         <v>-4</v>
       </c>
-    </row>
-    <row r="51" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT50">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A51" s="19" t="s">
         <v>293</v>
       </c>
@@ -14454,8 +14610,11 @@
       <c r="CS51">
         <v>-6.7249999999999996</v>
       </c>
-    </row>
-    <row r="52" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT51">
+        <v>-6.7249999999999996</v>
+      </c>
+    </row>
+    <row r="52" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A52" s="19" t="s">
         <v>294</v>
       </c>
@@ -14633,8 +14792,11 @@
       <c r="CS52">
         <v>-2.3250000000000002</v>
       </c>
-    </row>
-    <row r="53" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT52">
+        <v>-2.3250000000000002</v>
+      </c>
+    </row>
+    <row r="53" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A53" s="19" t="s">
         <v>295</v>
       </c>
@@ -14809,8 +14971,11 @@
       <c r="CS53">
         <v>9.1</v>
       </c>
-    </row>
-    <row r="54" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT53">
+        <v>9.1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A54" s="19" t="s">
         <v>296</v>
       </c>
@@ -14982,8 +15147,11 @@
       <c r="CS54">
         <v>12</v>
       </c>
-    </row>
-    <row r="55" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT54">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="55" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A55" s="19" t="s">
         <v>297</v>
       </c>
@@ -15152,8 +15320,11 @@
       <c r="CS55">
         <v>16.841666666666669</v>
       </c>
-    </row>
-    <row r="56" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT55">
+        <v>16.841666666666669</v>
+      </c>
+    </row>
+    <row r="56" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A56" s="19" t="s">
         <v>298</v>
       </c>
@@ -15319,8 +15490,11 @@
       <c r="CS56">
         <v>19.30833333333333</v>
       </c>
-    </row>
-    <row r="57" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT56">
+        <v>19.30833333333333</v>
+      </c>
+    </row>
+    <row r="57" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A57" s="19" t="s">
         <v>299</v>
       </c>
@@ -15483,8 +15657,11 @@
       <c r="CS57">
         <v>32.725000000000001</v>
       </c>
-    </row>
-    <row r="58" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT57">
+        <v>32.725000000000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A58" s="19" t="s">
         <v>300</v>
       </c>
@@ -15644,8 +15821,11 @@
       <c r="CS58">
         <v>53.141666666666673</v>
       </c>
-    </row>
-    <row r="59" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT58">
+        <v>53.141666666666673</v>
+      </c>
+    </row>
+    <row r="59" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A59" s="19" t="s">
         <v>301</v>
       </c>
@@ -15802,8 +15982,11 @@
       <c r="CS59">
         <v>64.416666666666657</v>
       </c>
-    </row>
-    <row r="60" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT59">
+        <v>64.416666666666657</v>
+      </c>
+    </row>
+    <row r="60" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A60" s="19" t="s">
         <v>302</v>
       </c>
@@ -15957,8 +16140,11 @@
       <c r="CS60">
         <v>71.241666666666674</v>
       </c>
-    </row>
-    <row r="61" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT60">
+        <v>71.241666666666674</v>
+      </c>
+    </row>
+    <row r="61" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A61" s="19" t="s">
         <v>303</v>
       </c>
@@ -16109,8 +16295,11 @@
       <c r="CS61">
         <v>82.85</v>
       </c>
-    </row>
-    <row r="62" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT61">
+        <v>82.85</v>
+      </c>
+    </row>
+    <row r="62" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A62" s="19" t="s">
         <v>304</v>
       </c>
@@ -16258,8 +16447,11 @@
       <c r="CS62">
         <v>65.241666666666674</v>
       </c>
-    </row>
-    <row r="63" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT62">
+        <v>65.241666666666674</v>
+      </c>
+    </row>
+    <row r="63" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A63" s="19" t="s">
         <v>305</v>
       </c>
@@ -16404,8 +16596,11 @@
       <c r="CS63">
         <v>46.391666666666673</v>
       </c>
-    </row>
-    <row r="64" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT63">
+        <v>46.391666666666673</v>
+      </c>
+    </row>
+    <row r="64" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A64" s="19" t="s">
         <v>306</v>
       </c>
@@ -16547,8 +16742,11 @@
       <c r="CS64">
         <v>37.733333333333327</v>
       </c>
-    </row>
-    <row r="65" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT64">
+        <v>37.733333333333327</v>
+      </c>
+    </row>
+    <row r="65" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A65" s="19" t="s">
         <v>307</v>
       </c>
@@ -16687,8 +16885,11 @@
       <c r="CS65">
         <v>22.8125</v>
       </c>
-    </row>
-    <row r="66" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT65">
+        <v>22.8125</v>
+      </c>
+    </row>
+    <row r="66" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A66" s="19" t="s">
         <v>308</v>
       </c>
@@ -16824,8 +17025,11 @@
       <c r="CS66">
         <v>11.7</v>
       </c>
-    </row>
-    <row r="67" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT66">
+        <v>11.7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A67" s="19" t="s">
         <v>309</v>
       </c>
@@ -16958,8 +17162,11 @@
       <c r="CS67">
         <v>2.1875</v>
       </c>
-    </row>
-    <row r="68" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT67">
+        <v>2.1875</v>
+      </c>
+    </row>
+    <row r="68" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A68" s="19" t="s">
         <v>310</v>
       </c>
@@ -17089,8 +17296,11 @@
       <c r="CS68">
         <v>-3.274999999999999</v>
       </c>
-    </row>
-    <row r="69" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT68">
+        <v>-3.274999999999999</v>
+      </c>
+    </row>
+    <row r="69" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A69" s="19" t="s">
         <v>311</v>
       </c>
@@ -17217,8 +17427,11 @@
       <c r="CS69">
         <v>-1.1499999999999999</v>
       </c>
-    </row>
-    <row r="70" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT69">
+        <v>-1.1499999999999999</v>
+      </c>
+    </row>
+    <row r="70" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A70" s="19" t="s">
         <v>312</v>
       </c>
@@ -17342,8 +17555,11 @@
       <c r="CS70">
         <v>-1.2749999999999999</v>
       </c>
-    </row>
-    <row r="71" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT70">
+        <v>-1.2749999999999999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A71" s="19" t="s">
         <v>313</v>
       </c>
@@ -17464,8 +17680,11 @@
       <c r="CS71">
         <v>-7.6</v>
       </c>
-    </row>
-    <row r="72" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT71">
+        <v>-7.6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A72" s="19" t="s">
         <v>314</v>
       </c>
@@ -17583,8 +17802,11 @@
       <c r="CS72">
         <v>-9.3625000000000007</v>
       </c>
-    </row>
-    <row r="73" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT72">
+        <v>-9.3625000000000007</v>
+      </c>
+    </row>
+    <row r="73" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A73" s="19" t="s">
         <v>315</v>
       </c>
@@ -17699,8 +17921,11 @@
       <c r="CS73">
         <v>-3.5249999999999999</v>
       </c>
-    </row>
-    <row r="74" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT73">
+        <v>-3.5249999999999999</v>
+      </c>
+    </row>
+    <row r="74" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A74" s="19" t="s">
         <v>316</v>
       </c>
@@ -17812,8 +18037,11 @@
       <c r="CS74">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="75" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT74">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A75" s="19" t="s">
         <v>317</v>
       </c>
@@ -17922,8 +18150,11 @@
       <c r="CS75">
         <v>-3.95</v>
       </c>
-    </row>
-    <row r="76" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT75">
+        <v>-3.95</v>
+      </c>
+    </row>
+    <row r="76" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A76" s="19" t="s">
         <v>318</v>
       </c>
@@ -18029,8 +18260,11 @@
       <c r="CS76">
         <v>-5.4083333333333332</v>
       </c>
-    </row>
-    <row r="77" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT76">
+        <v>-5.4083333333333332</v>
+      </c>
+    </row>
+    <row r="77" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A77" s="19" t="s">
         <v>319</v>
       </c>
@@ -18133,8 +18367,11 @@
       <c r="CS77">
         <v>-4.9333333333333336</v>
       </c>
-    </row>
-    <row r="78" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT77">
+        <v>-4.9333333333333336</v>
+      </c>
+    </row>
+    <row r="78" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A78" s="19" t="s">
         <v>320</v>
       </c>
@@ -18234,8 +18471,11 @@
       <c r="CS78">
         <v>-7.1833333333333336</v>
       </c>
-    </row>
-    <row r="79" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT78">
+        <v>-7.1833333333333336</v>
+      </c>
+    </row>
+    <row r="79" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A79" s="19" t="s">
         <v>321</v>
       </c>
@@ -18332,8 +18572,11 @@
       <c r="CS79">
         <v>-15.03333333333333</v>
       </c>
-    </row>
-    <row r="80" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT79">
+        <v>-15.03333333333333</v>
+      </c>
+    </row>
+    <row r="80" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A80" s="19" t="s">
         <v>322</v>
       </c>
@@ -18427,8 +18670,11 @@
       <c r="CS80">
         <v>-10.883333333333329</v>
       </c>
-    </row>
-    <row r="81" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT80">
+        <v>-10.883333333333329</v>
+      </c>
+    </row>
+    <row r="81" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A81" s="19" t="s">
         <v>323</v>
       </c>
@@ -18519,8 +18765,11 @@
       <c r="CS81">
         <v>-7.395833333333333</v>
       </c>
-    </row>
-    <row r="82" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT81">
+        <v>-7.395833333333333</v>
+      </c>
+    </row>
+    <row r="82" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A82" s="19" t="s">
         <v>324</v>
       </c>
@@ -18608,8 +18857,11 @@
       <c r="CS82">
         <v>-3.7666666666666662</v>
       </c>
-    </row>
-    <row r="83" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT82">
+        <v>-3.7666666666666662</v>
+      </c>
+    </row>
+    <row r="83" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A83" s="19" t="s">
         <v>325</v>
       </c>
@@ -18694,8 +18946,11 @@
       <c r="CS83">
         <v>-0.33333333333333298</v>
       </c>
-    </row>
-    <row r="84" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT83">
+        <v>-0.33333333333333298</v>
+      </c>
+    </row>
+    <row r="84" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A84" s="19" t="s">
         <v>326</v>
       </c>
@@ -18777,8 +19032,11 @@
       <c r="CS84">
         <v>-8.1083333333333343</v>
       </c>
-    </row>
-    <row r="85" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT84">
+        <v>-8.1083333333333343</v>
+      </c>
+    </row>
+    <row r="85" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A85" s="19" t="s">
         <v>327</v>
       </c>
@@ -18857,8 +19115,11 @@
       <c r="CS85">
         <v>-7.4166666666666661</v>
       </c>
-    </row>
-    <row r="86" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT85">
+        <v>-7.4166666666666661</v>
+      </c>
+    </row>
+    <row r="86" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A86" s="19" t="s">
         <v>328</v>
       </c>
@@ -18934,8 +19195,11 @@
       <c r="CS86">
         <v>-4.2476190476190476</v>
       </c>
-    </row>
-    <row r="87" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT86">
+        <v>-4.2476190476190476</v>
+      </c>
+    </row>
+    <row r="87" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A87" s="19" t="s">
         <v>329</v>
       </c>
@@ -19008,8 +19272,11 @@
       <c r="CS87">
         <v>-3.3142857142857149</v>
       </c>
-    </row>
-    <row r="88" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT87">
+        <v>-3.3142857142857149</v>
+      </c>
+    </row>
+    <row r="88" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A88" s="19" t="s">
         <v>330</v>
       </c>
@@ -19079,8 +19346,11 @@
       <c r="CS88">
         <v>-6.7</v>
       </c>
-    </row>
-    <row r="89" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT88">
+        <v>-6.7</v>
+      </c>
+    </row>
+    <row r="89" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A89" s="19" t="s">
         <v>331</v>
       </c>
@@ -19147,8 +19417,11 @@
       <c r="CS89">
         <v>3.35952380952381</v>
       </c>
-    </row>
-    <row r="90" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT89">
+        <v>3.35952380952381</v>
+      </c>
+    </row>
+    <row r="90" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A90" s="19" t="s">
         <v>332</v>
       </c>
@@ -19212,8 +19485,11 @@
       <c r="CS90">
         <v>5.4297619047619046</v>
       </c>
-    </row>
-    <row r="91" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT90">
+        <v>5.4297619047619046</v>
+      </c>
+    </row>
+    <row r="91" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A91" s="19" t="s">
         <v>333</v>
       </c>
@@ -19274,8 +19550,11 @@
       <c r="CS91">
         <v>8.9749999999999996</v>
       </c>
-    </row>
-    <row r="92" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT91">
+        <v>8.9749999999999996</v>
+      </c>
+    </row>
+    <row r="92" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A92" s="19" t="s">
         <v>334</v>
       </c>
@@ -19333,8 +19612,11 @@
       <c r="CS92">
         <v>11.483333333333331</v>
       </c>
-    </row>
-    <row r="93" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT92">
+        <v>11.483333333333331</v>
+      </c>
+    </row>
+    <row r="93" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A93" s="19" t="s">
         <v>335</v>
       </c>
@@ -19389,8 +19671,11 @@
       <c r="CS93">
         <v>6.4380952380952383</v>
       </c>
-    </row>
-    <row r="94" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT93">
+        <v>6.4380952380952383</v>
+      </c>
+    </row>
+    <row r="94" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A94" s="19" t="s">
         <v>336</v>
       </c>
@@ -19442,8 +19727,11 @@
       <c r="CS94">
         <v>5.8666666666666671</v>
       </c>
-    </row>
-    <row r="95" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT94">
+        <v>5.8666666666666671</v>
+      </c>
+    </row>
+    <row r="95" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A95" s="19" t="s">
         <v>337</v>
       </c>
@@ -19492,8 +19780,11 @@
       <c r="CS95">
         <v>4.1392857142857142</v>
       </c>
-    </row>
-    <row r="96" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT95">
+        <v>4.1392857142857142</v>
+      </c>
+    </row>
+    <row r="96" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A96" s="19" t="s">
         <v>338</v>
       </c>
@@ -19539,8 +19830,11 @@
       <c r="CS96">
         <v>0.20000000000000021</v>
       </c>
-    </row>
-    <row r="97" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT96">
+        <v>0.20000000000000021</v>
+      </c>
+    </row>
+    <row r="97" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A97" s="19" t="s">
         <v>339</v>
       </c>
@@ -19583,8 +19877,11 @@
       <c r="CS97">
         <v>-1.980952380952381</v>
       </c>
-    </row>
-    <row r="98" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT97">
+        <v>-1.980952380952381</v>
+      </c>
+    </row>
+    <row r="98" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A98" s="19" t="s">
         <v>340</v>
       </c>
@@ -19624,8 +19921,11 @@
       <c r="CS98">
         <v>-0.79166666666666707</v>
       </c>
-    </row>
-    <row r="99" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT98">
+        <v>-0.79166666666666707</v>
+      </c>
+    </row>
+    <row r="99" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A99" s="19" t="s">
         <v>341</v>
       </c>
@@ -19662,8 +19962,11 @@
       <c r="CS99">
         <v>-4.0999999999999996</v>
       </c>
-    </row>
-    <row r="100" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT99">
+        <v>-4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="100" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A100" s="19" t="s">
         <v>342</v>
       </c>
@@ -19697,8 +20000,11 @@
       <c r="CS100">
         <v>-6.5583333333333336</v>
       </c>
-    </row>
-    <row r="101" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT100">
+        <v>-6.5583333333333336</v>
+      </c>
+    </row>
+    <row r="101" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A101" s="19" t="s">
         <v>343</v>
       </c>
@@ -19729,8 +20035,11 @@
       <c r="CS101">
         <v>-5.8416666666666668</v>
       </c>
-    </row>
-    <row r="102" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT101">
+        <v>-5.8416666666666668</v>
+      </c>
+    </row>
+    <row r="102" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A102" s="19" t="s">
         <v>344</v>
       </c>
@@ -19758,8 +20067,11 @@
       <c r="CS102">
         <v>4.7125000000000004</v>
       </c>
-    </row>
-    <row r="103" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT102">
+        <v>4.7125000000000004</v>
+      </c>
+    </row>
+    <row r="103" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A103" s="19" t="s">
         <v>345</v>
       </c>
@@ -19784,8 +20096,11 @@
       <c r="CS103">
         <v>0.7488095238095237</v>
       </c>
-    </row>
-    <row r="104" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT103">
+        <v>0.7488095238095237</v>
+      </c>
+    </row>
+    <row r="104" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A104" s="19" t="s">
         <v>346</v>
       </c>
@@ -19807,8 +20122,11 @@
       <c r="CS104">
         <v>-1.33095238095238</v>
       </c>
-    </row>
-    <row r="105" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT104">
+        <v>-1.33095238095238</v>
+      </c>
+    </row>
+    <row r="105" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A105" s="19" t="s">
         <v>347</v>
       </c>
@@ -19827,8 +20145,11 @@
       <c r="CS105">
         <v>6.7</v>
       </c>
-    </row>
-    <row r="106" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT105">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="106" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A106" s="19">
         <v>43831</v>
       </c>
@@ -19844,8 +20165,11 @@
       <c r="CS106">
         <v>-3.095238095238095E-2</v>
       </c>
-    </row>
-    <row r="107" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT106">
+        <v>-3.095238095238095E-2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A107" s="19">
         <v>43922</v>
       </c>
@@ -19858,8 +20182,11 @@
       <c r="CS107">
         <v>35.61785714285714</v>
       </c>
-    </row>
-    <row r="108" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT107">
+        <v>35.61785714285714</v>
+      </c>
+    </row>
+    <row r="108" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A108" s="19">
         <v>44013</v>
       </c>
@@ -19869,13 +20196,27 @@
       <c r="CS108">
         <v>68.608333333333334</v>
       </c>
-    </row>
-    <row r="109" spans="1:97" x14ac:dyDescent="0.35">
+      <c r="CT108">
+        <v>68.608333333333334</v>
+      </c>
+    </row>
+    <row r="109" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A109" s="19">
         <v>44105</v>
       </c>
       <c r="CS109">
         <v>34.885714285714286</v>
+      </c>
+      <c r="CT109">
+        <v>34.885714285714286</v>
+      </c>
+    </row>
+    <row r="110" spans="1:98" x14ac:dyDescent="0.25">
+      <c r="A110" s="19">
+        <v>44197</v>
+      </c>
+      <c r="CT110">
+        <v>11.091666666666667</v>
       </c>
     </row>
   </sheetData>
@@ -19887,24 +20228,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B109"/>
+  <dimension ref="A1:B110"/>
   <sheetViews>
     <sheetView topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="A106" sqref="A106"/>
+      <selection activeCell="D116" sqref="D116"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="17">
         <v>34335</v>
       </c>
@@ -19912,7 +20253,7 @@
         <v>-8.8699999999999992</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="17">
         <v>34425</v>
       </c>
@@ -19920,7 +20261,7 @@
         <v>-8.8324999999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="17">
         <v>34516</v>
       </c>
@@ -19928,7 +20269,7 @@
         <v>-5.6375000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="17">
         <v>34608</v>
       </c>
@@ -19936,7 +20277,7 @@
         <v>-10.862500000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="17">
         <v>34700</v>
       </c>
@@ -19944,7 +20285,7 @@
         <v>-3.375</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="17">
         <v>34790</v>
       </c>
@@ -19952,7 +20293,7 @@
         <v>-4.6825000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="17">
         <v>34881</v>
       </c>
@@ -19960,7 +20301,7 @@
         <v>-1.2175</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="17">
         <v>34973</v>
       </c>
@@ -19968,7 +20309,7 @@
         <v>1.1325000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="17">
         <v>35065</v>
       </c>
@@ -19976,7 +20317,7 @@
         <v>5.9450000000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="17">
         <v>35156</v>
       </c>
@@ -19984,7 +20325,7 @@
         <v>2.4500000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="17">
         <v>35247</v>
       </c>
@@ -19992,7 +20333,7 @@
         <v>1.0249999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="17">
         <v>35339</v>
       </c>
@@ -20000,7 +20341,7 @@
         <v>-4.45</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="17">
         <v>35431</v>
       </c>
@@ -20008,7 +20349,7 @@
         <v>-2.1875</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="17">
         <v>35521</v>
       </c>
@@ -20016,7 +20357,7 @@
         <v>-4.3624999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="17">
         <v>35612</v>
       </c>
@@ -20024,7 +20365,7 @@
         <v>-5.25</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="17">
         <v>35704</v>
       </c>
@@ -20032,7 +20373,7 @@
         <v>-4.3499999999999996</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="17">
         <v>35796</v>
       </c>
@@ -20040,7 +20381,7 @@
         <v>-0.875</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="17">
         <v>35886</v>
       </c>
@@ -20048,7 +20389,7 @@
         <v>-5.4749999999999996</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="17">
         <v>35977</v>
       </c>
@@ -20056,7 +20397,7 @@
         <v>-1.3</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="17">
         <v>36069</v>
       </c>
@@ -20064,7 +20405,7 @@
         <v>23.925000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="17">
         <v>36161</v>
       </c>
@@ -20072,7 +20413,7 @@
         <v>6.9749999999999996</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="17">
         <v>36251</v>
       </c>
@@ -20080,7 +20421,7 @@
         <v>5.85</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="17">
         <v>36342</v>
       </c>
@@ -20088,7 +20429,7 @@
         <v>3.5750000000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="17">
         <v>36434</v>
       </c>
@@ -20096,7 +20437,7 @@
         <v>4.5250000000000004</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="17">
         <v>36526</v>
       </c>
@@ -20104,7 +20445,7 @@
         <v>7.3250000000000002</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="17">
         <v>36617</v>
       </c>
@@ -20112,7 +20453,7 @@
         <v>15.45</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="17">
         <v>36708</v>
       </c>
@@ -20120,7 +20461,7 @@
         <v>22.4</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="17">
         <v>36800</v>
       </c>
@@ -20128,7 +20469,7 @@
         <v>24.35</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="17">
         <v>36892</v>
       </c>
@@ -20136,7 +20477,7 @@
         <v>37.424999999999997</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="17">
         <v>36982</v>
       </c>
@@ -20144,7 +20485,7 @@
         <v>33.225000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="17">
         <v>37073</v>
       </c>
@@ -20152,7 +20493,7 @@
         <v>29.6</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="17">
         <v>37165</v>
       </c>
@@ -20160,7 +20501,7 @@
         <v>34.950000000000003</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="17">
         <v>37257</v>
       </c>
@@ -20168,7 +20509,7 @@
         <v>33.85</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="17">
         <v>37347</v>
       </c>
@@ -20176,7 +20517,7 @@
         <v>18.074999999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="17">
         <v>37438</v>
       </c>
@@ -20184,7 +20525,7 @@
         <v>14.074999999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="17">
         <v>37530</v>
       </c>
@@ -20192,7 +20533,7 @@
         <v>17.600000000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="17">
         <v>37622</v>
       </c>
@@ -20200,7 +20541,7 @@
         <v>15.125</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="17">
         <v>37712</v>
       </c>
@@ -20208,7 +20549,7 @@
         <v>11.275</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="17">
         <v>37803</v>
       </c>
@@ -20216,7 +20557,7 @@
         <v>5.6749999999999998</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="17">
         <v>37895</v>
       </c>
@@ -20224,7 +20565,7 @@
         <v>-0.45</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="17">
         <v>37987</v>
       </c>
@@ -20232,7 +20573,7 @@
         <v>-9.0500000000000007</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="17">
         <v>38078</v>
       </c>
@@ -20240,7 +20581,7 @@
         <v>-15.324999999999999</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="17">
         <v>38169</v>
       </c>
@@ -20248,7 +20589,7 @@
         <v>-9.6</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="17">
         <v>38261</v>
       </c>
@@ -20256,7 +20597,7 @@
         <v>-13.725</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="17">
         <v>38353</v>
       </c>
@@ -20264,7 +20605,7 @@
         <v>-17</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="17">
         <v>38443</v>
       </c>
@@ -20272,7 +20613,7 @@
         <v>-18.125</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="17">
         <v>38534</v>
       </c>
@@ -20280,7 +20621,7 @@
         <v>-10.175000000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="17">
         <v>38626</v>
       </c>
@@ -20288,7 +20629,7 @@
         <v>-5.75</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="17">
         <v>38718</v>
       </c>
@@ -20296,7 +20637,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="17">
         <v>38808</v>
       </c>
@@ -20304,7 +20645,7 @@
         <v>-6.7249999999999996</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="17">
         <v>38899</v>
       </c>
@@ -20312,7 +20653,7 @@
         <v>-2.3250000000000002</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="17">
         <v>38991</v>
       </c>
@@ -20320,7 +20661,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="17">
         <v>39083</v>
       </c>
@@ -20328,7 +20669,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="17">
         <v>39173</v>
       </c>
@@ -20336,7 +20677,7 @@
         <v>16.841666666666669</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="17">
         <v>39264</v>
       </c>
@@ -20344,7 +20685,7 @@
         <v>19.308333333333334</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="17">
         <v>39356</v>
       </c>
@@ -20352,7 +20693,7 @@
         <v>32.725000000000001</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="17">
         <v>39448</v>
       </c>
@@ -20360,7 +20701,7 @@
         <v>53.141666666666666</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="17">
         <v>39539</v>
       </c>
@@ -20368,7 +20709,7 @@
         <v>64.416666666666657</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="17">
         <v>39630</v>
       </c>
@@ -20376,7 +20717,7 @@
         <v>71.241666666666674</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="17">
         <v>39722</v>
       </c>
@@ -20384,7 +20725,7 @@
         <v>82.85</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="17">
         <v>39814</v>
       </c>
@@ -20392,7 +20733,7 @@
         <v>65.241666666666674</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="17">
         <v>39904</v>
       </c>
@@ -20400,7 +20741,7 @@
         <v>46.391666666666666</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="17">
         <v>39995</v>
       </c>
@@ -20408,7 +20749,7 @@
         <v>37.733333333333334</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="17">
         <v>40087</v>
       </c>
@@ -20416,7 +20757,7 @@
         <v>22.8125</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="17">
         <v>40179</v>
       </c>
@@ -20424,7 +20765,7 @@
         <v>11.7</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="17">
         <v>40269</v>
       </c>
@@ -20432,7 +20773,7 @@
         <v>2.1875</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="17">
         <v>40360</v>
       </c>
@@ -20440,7 +20781,7 @@
         <v>-3.2749999999999995</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="17">
         <v>40452</v>
       </c>
@@ -20448,7 +20789,7 @@
         <v>-1.1500000000000004</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="17">
         <v>40544</v>
       </c>
@@ -20456,7 +20797,7 @@
         <v>-1.2749999999999999</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="17">
         <v>40634</v>
       </c>
@@ -20464,7 +20805,7 @@
         <v>-7.6</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="17">
         <v>40725</v>
       </c>
@@ -20472,7 +20813,7 @@
         <v>-9.3625000000000007</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="17">
         <v>40817</v>
       </c>
@@ -20480,7 +20821,7 @@
         <v>-3.5250000000000004</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="17">
         <v>40909</v>
       </c>
@@ -20488,7 +20829,7 @@
         <v>1.2000000000000002</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="17">
         <v>41000</v>
       </c>
@@ -20496,7 +20837,7 @@
         <v>-3.95</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="17">
         <v>41091</v>
       </c>
@@ -20504,7 +20845,7 @@
         <v>-5.4083333333333332</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="17">
         <v>41183</v>
       </c>
@@ -20512,7 +20853,7 @@
         <v>-4.9333333333333336</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="17">
         <v>41275</v>
       </c>
@@ -20520,7 +20861,7 @@
         <v>-7.1833333333333336</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="17">
         <v>41365</v>
       </c>
@@ -20528,7 +20869,7 @@
         <v>-15.033333333333333</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="17">
         <v>41456</v>
       </c>
@@ -20536,7 +20877,7 @@
         <v>-10.883333333333333</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="17">
         <v>41548</v>
       </c>
@@ -20544,7 +20885,7 @@
         <v>-7.395833333333333</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="17">
         <v>41640</v>
       </c>
@@ -20552,7 +20893,7 @@
         <v>-3.7666666666666662</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="17">
         <v>41730</v>
       </c>
@@ -20560,7 +20901,7 @@
         <v>-0.33333333333333304</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="17">
         <v>41821</v>
       </c>
@@ -20568,7 +20909,7 @@
         <v>-8.1083333333333343</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="17">
         <v>41913</v>
       </c>
@@ -20576,7 +20917,7 @@
         <v>-7.4166666666666661</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="17">
         <v>42005</v>
       </c>
@@ -20584,7 +20925,7 @@
         <v>-4.2476190476190476</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="17">
         <v>42095</v>
       </c>
@@ -20592,7 +20933,7 @@
         <v>-3.3142857142857145</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="17">
         <v>42186</v>
       </c>
@@ -20600,7 +20941,7 @@
         <v>-6.7</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="17">
         <v>42278</v>
       </c>
@@ -20608,7 +20949,7 @@
         <v>3.35952380952381</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="17">
         <v>42370</v>
       </c>
@@ -20616,7 +20957,7 @@
         <v>5.4297619047619046</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="17">
         <v>42461</v>
       </c>
@@ -20624,7 +20965,7 @@
         <v>8.9749999999999996</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="17">
         <v>42552</v>
       </c>
@@ -20632,7 +20973,7 @@
         <v>11.483333333333333</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="17">
         <v>42644</v>
       </c>
@@ -20640,7 +20981,7 @@
         <v>6.4380952380952383</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="17">
         <v>42736</v>
       </c>
@@ -20648,7 +20989,7 @@
         <v>5.8666666666666671</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="17">
         <v>42826</v>
       </c>
@@ -20656,7 +20997,7 @@
         <v>4.1392857142857142</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="17">
         <v>42917</v>
       </c>
@@ -20664,7 +21005,7 @@
         <v>0.20000000000000018</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="17">
         <v>43009</v>
       </c>
@@ -20672,7 +21013,7 @@
         <v>-1.9809523809523812</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="17">
         <v>43101</v>
       </c>
@@ -20680,7 +21021,7 @@
         <v>-0.79166666666666707</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="17">
         <v>43191</v>
       </c>
@@ -20688,7 +21029,7 @@
         <v>-4.0999999999999996</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="17">
         <v>43282</v>
       </c>
@@ -20696,7 +21037,7 @@
         <v>-6.5583333333333336</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="17">
         <v>43374</v>
       </c>
@@ -20704,7 +21045,7 @@
         <v>-5.8416666666666668</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="17">
         <v>43466</v>
       </c>
@@ -20712,7 +21053,7 @@
         <v>4.7125000000000004</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="17">
         <v>43556</v>
       </c>
@@ -20720,7 +21061,7 @@
         <v>0.7488095238095237</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="17">
         <v>43647</v>
       </c>
@@ -20728,7 +21069,7 @@
         <v>-1.3309523809523802</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="17">
         <v>43739</v>
       </c>
@@ -20736,7 +21077,7 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="17">
         <v>43831</v>
       </c>
@@ -20744,7 +21085,7 @@
         <v>-3.0952380952380953E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="17">
         <v>43922</v>
       </c>
@@ -20752,7 +21093,7 @@
         <v>35.61785714285714</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="17">
         <v>44013</v>
       </c>
@@ -20760,12 +21101,20 @@
         <v>68.608333333333334</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="17">
         <v>44105</v>
       </c>
       <c r="B109">
         <v>34.885714285714286</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" s="17">
+        <v>44197</v>
+      </c>
+      <c r="B110">
+        <v>11.091666666666667</v>
       </c>
     </row>
   </sheetData>
@@ -20778,27 +21127,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:W140"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="I115" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W133" sqref="W133"/>
+      <selection pane="bottomRight" activeCell="K134" sqref="K134"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.1796875" style="4" customWidth="1"/>
-    <col min="2" max="8" width="5.26953125" style="4" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="5.26953125" style="6" customWidth="1"/>
-    <col min="10" max="10" width="5.26953125" style="4" customWidth="1"/>
-    <col min="11" max="11" width="6.1796875" style="6" customWidth="1"/>
-    <col min="12" max="14" width="5.26953125" style="4" customWidth="1"/>
-    <col min="15" max="15" width="5.26953125" style="8" customWidth="1"/>
-    <col min="16" max="28" width="5.26953125" style="4" customWidth="1"/>
-    <col min="29" max="16384" width="8.81640625" style="4"/>
+    <col min="1" max="1" width="7.140625" style="4" customWidth="1"/>
+    <col min="2" max="8" width="5.28515625" style="4" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="5.28515625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="5.28515625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="6.140625" style="6" customWidth="1"/>
+    <col min="12" max="14" width="5.28515625" style="4" customWidth="1"/>
+    <col min="15" max="15" width="5.28515625" style="8" customWidth="1"/>
+    <col min="16" max="28" width="5.28515625" style="4" customWidth="1"/>
+    <col min="29" max="16384" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>101</v>
       </c>
@@ -20848,7 +21197,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -20866,7 +21215,7 @@
       <c r="Q2" s="8"/>
       <c r="R2" s="8"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -20885,7 +21234,7 @@
       <c r="S3" s="8"/>
       <c r="V3" s="8"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
@@ -20903,7 +21252,7 @@
       <c r="R4" s="8"/>
       <c r="V4" s="8"/>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
@@ -20921,7 +21270,7 @@
       <c r="R5" s="8"/>
       <c r="V5" s="8"/>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -20939,7 +21288,7 @@
       <c r="R6" s="8"/>
       <c r="V6" s="8"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
@@ -20957,7 +21306,7 @@
       <c r="R7" s="8"/>
       <c r="V7" s="8"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
@@ -20975,7 +21324,7 @@
       <c r="R8" s="8"/>
       <c r="V8" s="8"/>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
@@ -20993,7 +21342,7 @@
       <c r="R9" s="8"/>
       <c r="V9" s="8"/>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
@@ -21011,7 +21360,7 @@
       <c r="R10" s="8"/>
       <c r="V10" s="8"/>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
@@ -21029,7 +21378,7 @@
       <c r="R11" s="8"/>
       <c r="V11" s="8"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
@@ -21047,7 +21396,7 @@
       <c r="R12" s="8"/>
       <c r="V12" s="8"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
@@ -21065,7 +21414,7 @@
       <c r="R13" s="8"/>
       <c r="V13" s="8"/>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>13</v>
       </c>
@@ -21083,7 +21432,7 @@
       <c r="R14" s="8"/>
       <c r="V14" s="8"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>14</v>
       </c>
@@ -21101,7 +21450,7 @@
       <c r="R15" s="8"/>
       <c r="V15" s="8"/>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>15</v>
       </c>
@@ -21119,7 +21468,7 @@
       <c r="R16" s="8"/>
       <c r="V16" s="8"/>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>16</v>
       </c>
@@ -21137,7 +21486,7 @@
       <c r="R17" s="8"/>
       <c r="V17" s="8"/>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>17</v>
       </c>
@@ -21155,7 +21504,7 @@
       <c r="R18" s="8"/>
       <c r="V18" s="8"/>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>18</v>
       </c>
@@ -21173,7 +21522,7 @@
       <c r="R19" s="8"/>
       <c r="V19" s="8"/>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>19</v>
       </c>
@@ -21191,7 +21540,7 @@
       <c r="R20" s="8"/>
       <c r="V20" s="8"/>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>20</v>
       </c>
@@ -21209,7 +21558,7 @@
       <c r="R21" s="8"/>
       <c r="V21" s="8"/>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>21</v>
       </c>
@@ -21227,7 +21576,7 @@
       <c r="R22" s="8"/>
       <c r="V22" s="8"/>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>22</v>
       </c>
@@ -21245,7 +21594,7 @@
       <c r="R23" s="8"/>
       <c r="V23" s="8"/>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>23</v>
       </c>
@@ -21263,7 +21612,7 @@
       <c r="R24" s="8"/>
       <c r="V24" s="8"/>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>24</v>
       </c>
@@ -21281,7 +21630,7 @@
       <c r="R25" s="8"/>
       <c r="V25" s="8"/>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>25</v>
       </c>
@@ -21299,7 +21648,7 @@
       <c r="R26" s="8"/>
       <c r="V26" s="8"/>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>26</v>
       </c>
@@ -21317,7 +21666,7 @@
       <c r="R27" s="8"/>
       <c r="V27" s="8"/>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>27</v>
       </c>
@@ -21335,7 +21684,7 @@
       <c r="R28" s="8"/>
       <c r="V28" s="8"/>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>28</v>
       </c>
@@ -21353,7 +21702,7 @@
       <c r="R29" s="8"/>
       <c r="V29" s="8"/>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>29</v>
       </c>
@@ -21371,7 +21720,7 @@
       <c r="R30" s="8"/>
       <c r="V30" s="8"/>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>30</v>
       </c>
@@ -21389,7 +21738,7 @@
       <c r="R31" s="8"/>
       <c r="V31" s="8"/>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>31</v>
       </c>
@@ -21407,7 +21756,7 @@
       <c r="R32" s="8"/>
       <c r="V32" s="8"/>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>32</v>
       </c>
@@ -21425,7 +21774,7 @@
       <c r="R33" s="8"/>
       <c r="V33" s="8"/>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>33</v>
       </c>
@@ -21443,7 +21792,7 @@
       <c r="R34" s="8"/>
       <c r="V34" s="8"/>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>34</v>
       </c>
@@ -21461,7 +21810,7 @@
       <c r="R35" s="8"/>
       <c r="V35" s="8"/>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>35</v>
       </c>
@@ -21479,7 +21828,7 @@
       <c r="R36" s="8"/>
       <c r="V36" s="8"/>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>36</v>
       </c>
@@ -21497,7 +21846,7 @@
       <c r="R37" s="8"/>
       <c r="V37" s="8"/>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>37</v>
       </c>
@@ -21515,7 +21864,7 @@
       <c r="R38" s="8"/>
       <c r="V38" s="8"/>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>38</v>
       </c>
@@ -21533,7 +21882,7 @@
       <c r="R39" s="8"/>
       <c r="V39" s="8"/>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>39</v>
       </c>
@@ -21551,7 +21900,7 @@
       <c r="R40" s="8"/>
       <c r="V40" s="8"/>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>40</v>
       </c>
@@ -21569,7 +21918,7 @@
       <c r="R41" s="8"/>
       <c r="V41" s="8"/>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>41</v>
       </c>
@@ -21587,7 +21936,7 @@
       <c r="R42" s="8"/>
       <c r="V42" s="8"/>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>42</v>
       </c>
@@ -21605,7 +21954,7 @@
       <c r="R43" s="8"/>
       <c r="V43" s="8"/>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>43</v>
       </c>
@@ -21623,7 +21972,7 @@
       <c r="R44" s="8"/>
       <c r="V44" s="8"/>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>44</v>
       </c>
@@ -21641,7 +21990,7 @@
       <c r="R45" s="8"/>
       <c r="V45" s="8"/>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>45</v>
       </c>
@@ -21659,7 +22008,7 @@
       <c r="R46" s="8"/>
       <c r="V46" s="8"/>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>46</v>
       </c>
@@ -21677,7 +22026,7 @@
       <c r="R47" s="8"/>
       <c r="V47" s="8"/>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>47</v>
       </c>
@@ -21695,7 +22044,7 @@
       <c r="R48" s="8"/>
       <c r="V48" s="8"/>
     </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>48</v>
       </c>
@@ -21713,7 +22062,7 @@
       <c r="R49" s="8"/>
       <c r="V49" s="8"/>
     </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>49</v>
       </c>
@@ -21731,7 +22080,7 @@
       <c r="R50" s="8"/>
       <c r="V50" s="8"/>
     </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>50</v>
       </c>
@@ -21749,7 +22098,7 @@
       <c r="R51" s="8"/>
       <c r="V51" s="8"/>
     </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>51</v>
       </c>
@@ -21767,7 +22116,7 @@
       <c r="R52" s="8"/>
       <c r="V52" s="8"/>
     </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>52</v>
       </c>
@@ -21785,7 +22134,7 @@
       <c r="R53" s="8"/>
       <c r="V53" s="8"/>
     </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>53</v>
       </c>
@@ -21823,7 +22172,7 @@
       <c r="R54" s="8"/>
       <c r="V54" s="8"/>
     </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>54</v>
       </c>
@@ -21853,7 +22202,7 @@
       <c r="R55" s="8"/>
       <c r="V55" s="8"/>
     </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>55</v>
       </c>
@@ -21883,7 +22232,7 @@
       <c r="R56" s="8"/>
       <c r="V56" s="8"/>
     </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>56</v>
       </c>
@@ -21913,7 +22262,7 @@
       <c r="R57" s="8"/>
       <c r="V57" s="8"/>
     </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>57</v>
       </c>
@@ -21943,7 +22292,7 @@
       <c r="R58" s="8"/>
       <c r="V58" s="8"/>
     </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>58</v>
       </c>
@@ -21973,7 +22322,7 @@
       <c r="R59" s="8"/>
       <c r="V59" s="8"/>
     </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>59</v>
       </c>
@@ -22003,7 +22352,7 @@
       <c r="R60" s="8"/>
       <c r="V60" s="8"/>
     </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>60</v>
       </c>
@@ -22033,7 +22382,7 @@
       <c r="R61" s="8"/>
       <c r="V61" s="8"/>
     </row>
-    <row r="62" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>61</v>
       </c>
@@ -22089,7 +22438,7 @@
       </c>
       <c r="V62" s="8"/>
     </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>62</v>
       </c>
@@ -22120,7 +22469,7 @@
       <c r="R63" s="8"/>
       <c r="V63" s="8"/>
     </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>63</v>
       </c>
@@ -22150,7 +22499,7 @@
       <c r="R64" s="8"/>
       <c r="V64" s="8"/>
     </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>64</v>
       </c>
@@ -22177,7 +22526,7 @@
       <c r="R65" s="8"/>
       <c r="V65" s="8"/>
     </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>65</v>
       </c>
@@ -22204,7 +22553,7 @@
       <c r="R66" s="8"/>
       <c r="V66" s="8"/>
     </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>66</v>
       </c>
@@ -22231,7 +22580,7 @@
       <c r="R67" s="8"/>
       <c r="V67" s="8"/>
     </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>67</v>
       </c>
@@ -22258,7 +22607,7 @@
       <c r="R68" s="8"/>
       <c r="V68" s="8"/>
     </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>68</v>
       </c>
@@ -22285,7 +22634,7 @@
       <c r="R69" s="8"/>
       <c r="V69" s="8"/>
     </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
       <c r="E70" s="5"/>
@@ -22296,7 +22645,7 @@
       <c r="R70" s="8"/>
       <c r="V70" s="8"/>
     </row>
-    <row r="71" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C71" s="5"/>
       <c r="D71" s="5"/>
       <c r="E71" s="5"/>
@@ -22327,7 +22676,7 @@
       </c>
       <c r="V71" s="8"/>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>69</v>
       </c>
@@ -22359,7 +22708,7 @@
       <c r="T72" s="15"/>
       <c r="U72" s="15"/>
     </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
       <c r="K73" s="12"/>
       <c r="L73" s="13" t="s">
         <v>109</v>
@@ -22383,7 +22732,7 @@
       <c r="T73" s="15"/>
       <c r="U73" s="15"/>
     </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>70</v>
       </c>
@@ -22415,7 +22764,7 @@
       <c r="T74" s="15"/>
       <c r="U74" s="15"/>
     </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
       <c r="L75" s="13" t="s">
         <v>109</v>
       </c>
@@ -22438,7 +22787,7 @@
       <c r="T75" s="15"/>
       <c r="U75" s="15"/>
     </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>71</v>
       </c>
@@ -22470,7 +22819,7 @@
       <c r="T76" s="15"/>
       <c r="U76" s="15"/>
     </row>
-    <row r="77" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:22" x14ac:dyDescent="0.25">
       <c r="L77" s="13" t="s">
         <v>109</v>
       </c>
@@ -22493,7 +22842,7 @@
       <c r="T77" s="15"/>
       <c r="U77" s="15"/>
     </row>
-    <row r="78" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>72</v>
       </c>
@@ -22525,7 +22874,7 @@
       <c r="T78" s="15"/>
       <c r="U78" s="15"/>
     </row>
-    <row r="79" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:22" x14ac:dyDescent="0.25">
       <c r="L79" s="13" t="s">
         <v>109</v>
       </c>
@@ -22548,7 +22897,7 @@
       <c r="T79" s="15"/>
       <c r="U79" s="15"/>
     </row>
-    <row r="80" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>73</v>
       </c>
@@ -22579,7 +22928,7 @@
       <c r="T80" s="15"/>
       <c r="U80" s="15"/>
     </row>
-    <row r="81" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:21" x14ac:dyDescent="0.25">
       <c r="L81" s="13" t="s">
         <v>109</v>
       </c>
@@ -22602,7 +22951,7 @@
       <c r="T81" s="15"/>
       <c r="U81" s="15"/>
     </row>
-    <row r="82" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>74</v>
       </c>
@@ -22634,7 +22983,7 @@
       <c r="T82" s="15"/>
       <c r="U82" s="15"/>
     </row>
-    <row r="83" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:21" x14ac:dyDescent="0.25">
       <c r="L83" s="13" t="s">
         <v>109</v>
       </c>
@@ -22657,7 +23006,7 @@
       <c r="T83" s="15"/>
       <c r="U83" s="15"/>
     </row>
-    <row r="84" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
         <v>75</v>
       </c>
@@ -22693,7 +23042,7 @@
       <c r="T84" s="15"/>
       <c r="U84" s="15"/>
     </row>
-    <row r="85" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:21" x14ac:dyDescent="0.25">
       <c r="L85" s="13" t="s">
         <v>109</v>
       </c>
@@ -22716,7 +23065,7 @@
       <c r="T85" s="15"/>
       <c r="U85" s="15"/>
     </row>
-    <row r="86" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>76</v>
       </c>
@@ -22752,7 +23101,7 @@
       <c r="T86" s="15"/>
       <c r="U86" s="15"/>
     </row>
-    <row r="87" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:21" x14ac:dyDescent="0.25">
       <c r="L87" s="13" t="s">
         <v>109</v>
       </c>
@@ -22775,7 +23124,7 @@
       <c r="T87" s="15"/>
       <c r="U87" s="15"/>
     </row>
-    <row r="88" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
         <v>77</v>
       </c>
@@ -22811,7 +23160,7 @@
       <c r="T88" s="15"/>
       <c r="U88" s="15"/>
     </row>
-    <row r="89" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:21" x14ac:dyDescent="0.25">
       <c r="L89" s="13" t="s">
         <v>109</v>
       </c>
@@ -22834,7 +23183,7 @@
       <c r="T89" s="15"/>
       <c r="U89" s="15"/>
     </row>
-    <row r="90" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
         <v>78</v>
       </c>
@@ -22870,7 +23219,7 @@
       <c r="T90" s="15"/>
       <c r="U90" s="15"/>
     </row>
-    <row r="91" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:21" x14ac:dyDescent="0.25">
       <c r="L91" s="13" t="s">
         <v>109</v>
       </c>
@@ -22893,7 +23242,7 @@
       <c r="T91" s="15"/>
       <c r="U91" s="15"/>
     </row>
-    <row r="92" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
         <v>79</v>
       </c>
@@ -22929,7 +23278,7 @@
       <c r="T92" s="15"/>
       <c r="U92" s="15"/>
     </row>
-    <row r="93" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:21" x14ac:dyDescent="0.25">
       <c r="L93" s="13" t="s">
         <v>109</v>
       </c>
@@ -22955,7 +23304,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="94" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
         <v>80</v>
       </c>
@@ -22992,7 +23341,7 @@
         <v>-9.9999999999999645E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:21" x14ac:dyDescent="0.25">
       <c r="L95" s="13" t="s">
         <v>109</v>
       </c>
@@ -23020,7 +23369,7 @@
       <c r="T95" s="15"/>
       <c r="U95" s="15"/>
     </row>
-    <row r="96" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
         <v>81</v>
       </c>
@@ -23060,7 +23409,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="97" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:23" x14ac:dyDescent="0.25">
       <c r="L97" s="13" t="s">
         <v>109</v>
       </c>
@@ -23086,7 +23435,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="98" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
         <v>82</v>
       </c>
@@ -23127,7 +23476,7 @@
         <v>42.900000000000006</v>
       </c>
     </row>
-    <row r="99" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:23" x14ac:dyDescent="0.25">
       <c r="L99" s="13" t="s">
         <v>109</v>
       </c>
@@ -23153,7 +23502,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="100" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
         <v>83</v>
       </c>
@@ -23194,7 +23543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:23" x14ac:dyDescent="0.25">
       <c r="L101" s="13" t="s">
         <v>109</v>
       </c>
@@ -23220,7 +23569,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="102" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
         <v>84</v>
       </c>
@@ -23261,7 +23610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:23" x14ac:dyDescent="0.25">
       <c r="L103" s="13" t="s">
         <v>109</v>
       </c>
@@ -23299,7 +23648,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="104" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
         <v>85</v>
       </c>
@@ -23356,7 +23705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:23" x14ac:dyDescent="0.25">
       <c r="L105" s="13" t="s">
         <v>109</v>
       </c>
@@ -23394,7 +23743,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="106" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
         <v>86</v>
       </c>
@@ -23451,7 +23800,7 @@
         <v>16.7</v>
       </c>
     </row>
-    <row r="107" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:23" x14ac:dyDescent="0.25">
       <c r="L107" s="13" t="s">
         <v>109</v>
       </c>
@@ -23489,7 +23838,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="108" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
         <v>87</v>
       </c>
@@ -23546,7 +23895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
         <v>88</v>
       </c>
@@ -23603,7 +23952,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="110" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
         <v>89</v>
       </c>
@@ -23660,7 +24009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:23" x14ac:dyDescent="0.25">
       <c r="L111" s="13" t="s">
         <v>109</v>
       </c>
@@ -23698,7 +24047,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="112" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
         <v>90</v>
       </c>
@@ -23751,7 +24100,7 @@
         <v>-5.4</v>
       </c>
     </row>
-    <row r="113" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:23" x14ac:dyDescent="0.25">
       <c r="L113" s="13" t="s">
         <v>109</v>
       </c>
@@ -23789,7 +24138,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="114" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
         <v>91</v>
       </c>
@@ -23846,7 +24195,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="115" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:23" x14ac:dyDescent="0.25">
       <c r="L115" s="13" t="s">
         <v>109</v>
       </c>
@@ -23884,7 +24233,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="116" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
         <v>92</v>
       </c>
@@ -23941,7 +24290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:23" x14ac:dyDescent="0.25">
       <c r="L117" s="13" t="s">
         <v>109</v>
       </c>
@@ -23979,12 +24328,12 @@
         <v>141</v>
       </c>
     </row>
-    <row r="118" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
         <v>93</v>
       </c>
       <c r="K118" s="6">
-        <f t="shared" ref="K118:K133" si="3">AVERAGE(L118:M118,AVERAGE(N118:P118),AVERAGE(Q118:W118))</f>
+        <f t="shared" ref="K118:K134" si="3">AVERAGE(L118:M118,AVERAGE(N118:P118),AVERAGE(Q118:W118))</f>
         <v>5.8666666666666671</v>
       </c>
       <c r="L118" s="4">
@@ -24036,7 +24385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
         <v>94</v>
       </c>
@@ -24093,7 +24442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
         <v>95</v>
       </c>
@@ -24146,7 +24495,7 @@
         <v>-3.4</v>
       </c>
     </row>
-    <row r="121" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
         <v>96</v>
       </c>
@@ -24203,7 +24552,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="122" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
         <v>97</v>
       </c>
@@ -24256,7 +24605,7 @@
         <v>-2.1</v>
       </c>
     </row>
-    <row r="123" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="s">
         <v>98</v>
       </c>
@@ -24313,7 +24662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
         <v>99</v>
       </c>
@@ -24370,7 +24719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
         <v>100</v>
       </c>
@@ -24423,7 +24772,7 @@
         <v>-3.6999999999999997</v>
       </c>
     </row>
-    <row r="126" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
         <v>144</v>
       </c>
@@ -24476,7 +24825,7 @@
         <v>-1.8</v>
       </c>
     </row>
-    <row r="127" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="s">
         <v>145</v>
       </c>
@@ -24533,7 +24882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="s">
         <v>146</v>
       </c>
@@ -24589,7 +24938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="s">
         <v>147</v>
       </c>
@@ -24646,7 +24995,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="130" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
         <v>148</v>
       </c>
@@ -24703,7 +25052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="s">
         <v>149</v>
       </c>
@@ -24760,7 +25109,7 @@
         <v>14.3</v>
       </c>
     </row>
-    <row r="132" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
         <v>349</v>
       </c>
@@ -24817,7 +25166,7 @@
         <v>42.900000000000006</v>
       </c>
     </row>
-    <row r="133" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A133" s="4" t="s">
         <v>351</v>
       </c>
@@ -24874,25 +25223,79 @@
         <v>33.299999999999997</v>
       </c>
     </row>
-    <row r="134" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="O134" s="4"/>
-    </row>
-    <row r="135" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A134" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="K134" s="6">
+        <f t="shared" si="3"/>
+        <v>11.091666666666667</v>
+      </c>
+      <c r="L134" s="4">
+        <f>17.8-12.3</f>
+        <v>5.5</v>
+      </c>
+      <c r="M134" s="4">
+        <f>17.1-5.7</f>
+        <v>11.400000000000002</v>
+      </c>
+      <c r="N134" s="4">
+        <f>2.9+24.6-1.4</f>
+        <v>26.1</v>
+      </c>
+      <c r="O134" s="4">
+        <f>1.4+27.8</f>
+        <v>29.2</v>
+      </c>
+      <c r="P134" s="4">
+        <f>20.8</f>
+        <v>20.8</v>
+      </c>
+      <c r="Q134" s="4">
+        <f>3.2-6.5</f>
+        <v>-3.3</v>
+      </c>
+      <c r="R134" s="4">
+        <f>1.7-1.7</f>
+        <v>0</v>
+      </c>
+      <c r="S134" s="4">
+        <f>5-5</f>
+        <v>0</v>
+      </c>
+      <c r="T134" s="4">
+        <f>6.7-8.3</f>
+        <v>-1.6000000000000005</v>
+      </c>
+      <c r="U134" s="4">
+        <f>8.9-5.4</f>
+        <v>3.5</v>
+      </c>
+      <c r="V134" s="4">
+        <f>5.4-3.6</f>
+        <v>1.8000000000000003</v>
+      </c>
+      <c r="W134" s="4">
+        <f>14.3</f>
+        <v>14.3</v>
+      </c>
+    </row>
+    <row r="135" spans="1:23" x14ac:dyDescent="0.25">
       <c r="O135" s="4"/>
     </row>
-    <row r="136" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:23" x14ac:dyDescent="0.25">
       <c r="O136" s="4"/>
     </row>
-    <row r="137" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:23" x14ac:dyDescent="0.25">
       <c r="O137" s="4"/>
     </row>
-    <row r="138" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:23" x14ac:dyDescent="0.25">
       <c r="O138" s="4"/>
     </row>
-    <row r="139" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:23" x14ac:dyDescent="0.25">
       <c r="O139" s="4"/>
     </row>
-    <row r="140" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:23" x14ac:dyDescent="0.25">
       <c r="O140" s="4"/>
     </row>
   </sheetData>

</xml_diff>